<commit_message>
v6 and v7 eval results
</commit_message>
<xml_diff>
--- a/evaluation/results_by_data_split.xlsx
+++ b/evaluation/results_by_data_split.xlsx
@@ -8,19 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yufeizhao/Desktop/11667MiniProject/11667-NLP2SQL/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69B26574-0AD5-034C-8534-C9B58052C094}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA5B968-A8F9-A34A-91E4-545B63CD127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2060" yWindow="-19500" windowWidth="28040" windowHeight="17440" activeTab="7" xr2:uid="{44081516-0D10-9B41-9157-44A5B55A14F9}"/>
+    <workbookView xWindow="-1700" yWindow="-20560" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{44081516-0D10-9B41-9157-44A5B55A14F9}"/>
   </bookViews>
   <sheets>
     <sheet name="train_sql2sql" sheetId="1" r:id="rId1"/>
     <sheet name="val_sql2sql" sheetId="2" r:id="rId2"/>
     <sheet name="test_sql2sql" sheetId="3" r:id="rId3"/>
-    <sheet name="ptv2_eval_sql2sql" sheetId="4" r:id="rId4"/>
-    <sheet name="ptv3_eval_train_sql2sql" sheetId="6" r:id="rId5"/>
-    <sheet name="ptv3_eval_test_sql2sql" sheetId="7" r:id="rId6"/>
+    <sheet name="eval_train_sql2sql" sheetId="6" r:id="rId4"/>
+    <sheet name="eval_test_sql2sql" sheetId="7" r:id="rId5"/>
+    <sheet name="eval_res2res" sheetId="8" r:id="rId6"/>
     <sheet name="ptv2_eval_res2res" sheetId="5" r:id="rId7"/>
-    <sheet name="ptv3_eval_res2res" sheetId="8" r:id="rId8"/>
+    <sheet name="ptv2_eval_sql2sql" sheetId="4" r:id="rId8"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="91" uniqueCount="17">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="25">
   <si>
     <t>total queries</t>
   </si>
@@ -87,6 +87,12 @@
     <t>promptv3_codellama_v5</t>
   </si>
   <si>
+    <t>promptv3_codellama_v6</t>
+  </si>
+  <si>
+    <t>promptv3_codellama_v7</t>
+  </si>
+  <si>
     <t>eval_test</t>
   </si>
   <si>
@@ -95,12 +101,30 @@
   <si>
     <t>data_split</t>
   </si>
+  <si>
+    <t>promptv3_codellama_v7.1</t>
+  </si>
+  <si>
+    <t>promptv3_codellama_v7.2</t>
+  </si>
+  <si>
+    <t>promptv3_codellama_v7.3</t>
+  </si>
+  <si>
+    <t>promptv3_codellama_v7.4</t>
+  </si>
+  <si>
+    <t>promptv3_codellama_v7.5</t>
+  </si>
+  <si>
+    <t>promptv3_codellama_v7.6</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -116,24 +140,25 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="12"/>
+      <color rgb="FFFF0000"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="5">
+  <fills count="7">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="7" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
     </fill>
     <fill>
       <patternFill patternType="solid">
@@ -147,8 +172,26 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="8" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="3" tint="0.89999084444715716"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="14">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -323,11 +366,22 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="33">
+  <cellXfs count="49">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -410,6 +464,15 @@
     <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -423,6 +486,45 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -762,7 +864,7 @@
   <dimension ref="B2:H8"/>
   <sheetViews>
     <sheetView zoomScale="137" workbookViewId="0">
-      <selection activeCell="I11" sqref="I11"/>
+      <selection activeCell="H12" sqref="H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -931,15 +1033,15 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C775F-3A5B-8346-B68B-D75012605A96}">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:H16"/>
   <sheetViews>
-    <sheetView zoomScale="160" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
+    <sheetView zoomScale="157" workbookViewId="0">
+      <selection activeCell="H10" sqref="H10:H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
     <col min="3" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1092,26 +1194,211 @@
         <v>3.02</v>
       </c>
     </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3">
+        <v>250</v>
+      </c>
+      <c r="D9" s="3">
+        <v>118</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="F9" s="3">
+        <v>250</v>
+      </c>
+      <c r="G9" s="3">
+        <v>907</v>
+      </c>
+      <c r="H9" s="3">
+        <v>3.63</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>250</v>
+      </c>
+      <c r="D10" s="3">
+        <v>116</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.46400000000000002</v>
+      </c>
+      <c r="F10" s="3">
+        <v>250</v>
+      </c>
+      <c r="G10" s="3">
+        <v>862</v>
+      </c>
+      <c r="H10" s="3">
+        <v>3.45</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3">
+        <v>250</v>
+      </c>
+      <c r="D11" s="3">
+        <v>124</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.496</v>
+      </c>
+      <c r="F11" s="3">
+        <v>250</v>
+      </c>
+      <c r="G11" s="3">
+        <v>838</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3">
+        <v>250</v>
+      </c>
+      <c r="D12" s="3">
+        <v>126</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0.504</v>
+      </c>
+      <c r="F12" s="3">
+        <v>250</v>
+      </c>
+      <c r="G12" s="3">
+        <v>869</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3">
+        <v>250</v>
+      </c>
+      <c r="D13" s="3">
+        <v>123</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="F13" s="3">
+        <v>250</v>
+      </c>
+      <c r="G13" s="3">
+        <v>850</v>
+      </c>
+      <c r="H13" s="28">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3">
+        <v>250</v>
+      </c>
+      <c r="D14" s="3">
+        <v>124</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.496</v>
+      </c>
+      <c r="F14" s="3">
+        <v>250</v>
+      </c>
+      <c r="G14" s="3">
+        <v>844</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3">
+        <v>250</v>
+      </c>
+      <c r="D15" s="3">
+        <v>108</v>
+      </c>
+      <c r="E15" s="13">
+        <v>0.432</v>
+      </c>
+      <c r="F15" s="3">
+        <v>250</v>
+      </c>
+      <c r="G15" s="3">
+        <v>966</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3">
+        <v>250</v>
+      </c>
+      <c r="D16" s="3">
+        <v>109</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.436</v>
+      </c>
+      <c r="F16" s="3">
+        <v>250</v>
+      </c>
+      <c r="G16" s="3">
+        <v>967</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3.87</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82A48FE-26B2-E846-83D1-3D5B61BC4083}">
-  <dimension ref="B2:H8"/>
+  <dimension ref="B2:H16"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+      <selection activeCell="F20" sqref="F20"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
     <col min="3" max="8" width="12.83203125" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1264,16 +1551,1305 @@
         <v>3.19</v>
       </c>
     </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="14" t="s">
+        <v>14</v>
+      </c>
+      <c r="C9" s="3">
+        <v>250</v>
+      </c>
+      <c r="D9" s="3">
+        <v>121</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.48399999999999999</v>
+      </c>
+      <c r="F9" s="3">
+        <v>250</v>
+      </c>
+      <c r="G9" s="3">
+        <v>925</v>
+      </c>
+      <c r="H9" s="28">
+        <v>3.7</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="14" t="s">
+        <v>15</v>
+      </c>
+      <c r="C10" s="3">
+        <v>250</v>
+      </c>
+      <c r="D10" s="3">
+        <v>127</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.50800000000000001</v>
+      </c>
+      <c r="F10" s="3">
+        <v>250</v>
+      </c>
+      <c r="G10" s="29">
+        <v>890</v>
+      </c>
+      <c r="H10" s="29">
+        <v>3.56</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="14" t="s">
+        <v>19</v>
+      </c>
+      <c r="C11" s="3">
+        <v>250</v>
+      </c>
+      <c r="D11" s="3">
+        <v>124</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.496</v>
+      </c>
+      <c r="F11" s="3">
+        <v>250</v>
+      </c>
+      <c r="G11" s="3">
+        <v>899</v>
+      </c>
+      <c r="H11" s="28">
+        <v>3.6</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="14" t="s">
+        <v>20</v>
+      </c>
+      <c r="C12" s="3">
+        <v>250</v>
+      </c>
+      <c r="D12" s="3">
+        <v>132</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0.52800000000000002</v>
+      </c>
+      <c r="F12" s="3">
+        <v>250</v>
+      </c>
+      <c r="G12" s="3">
+        <v>869</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" s="3">
+        <v>250</v>
+      </c>
+      <c r="D13" s="3">
+        <v>125</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F13" s="3">
+        <v>250</v>
+      </c>
+      <c r="G13" s="3">
+        <v>876</v>
+      </c>
+      <c r="H13" s="28">
+        <v>3.5</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="14" t="s">
+        <v>22</v>
+      </c>
+      <c r="C14" s="3">
+        <v>250</v>
+      </c>
+      <c r="D14" s="3">
+        <v>138</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.55200000000000005</v>
+      </c>
+      <c r="F14" s="3">
+        <v>250</v>
+      </c>
+      <c r="G14" s="3">
+        <v>840</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="14" t="s">
+        <v>23</v>
+      </c>
+      <c r="C15" s="3">
+        <v>250</v>
+      </c>
+      <c r="D15" s="29">
+        <v>125</v>
+      </c>
+      <c r="E15" s="30">
+        <v>0.5</v>
+      </c>
+      <c r="F15" s="3">
+        <v>250</v>
+      </c>
+      <c r="G15" s="3">
+        <v>935</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3.74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="14" t="s">
+        <v>24</v>
+      </c>
+      <c r="C16" s="3">
+        <v>250</v>
+      </c>
+      <c r="D16" s="3">
+        <v>125</v>
+      </c>
+      <c r="E16" s="13">
+        <v>0.5</v>
+      </c>
+      <c r="F16" s="3">
+        <v>250</v>
+      </c>
+      <c r="G16" s="3">
+        <v>912</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3.65</v>
+      </c>
+    </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
   </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA613D23-B9DE-0542-95AA-364F896410C8}">
+  <dimension ref="B2:H14"/>
+  <sheetViews>
+    <sheetView zoomScale="150" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="3"/>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>150</v>
+      </c>
+      <c r="D4" s="3">
+        <v>5</v>
+      </c>
+      <c r="E4" s="13">
+        <v>3.3300000000000003E-2</v>
+      </c>
+      <c r="F4" s="3">
+        <v>150</v>
+      </c>
+      <c r="G4" s="3">
+        <v>1640</v>
+      </c>
+      <c r="H4" s="3">
+        <v>10.93</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>150</v>
+      </c>
+      <c r="D5" s="3">
+        <v>23</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.15329999999999999</v>
+      </c>
+      <c r="F5" s="3">
+        <v>150</v>
+      </c>
+      <c r="G5" s="3">
+        <v>283</v>
+      </c>
+      <c r="H5" s="3">
+        <v>1.89</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <v>150</v>
+      </c>
+      <c r="D6" s="3">
+        <v>9</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.06</v>
+      </c>
+      <c r="F6" s="3">
+        <v>150</v>
+      </c>
+      <c r="G6" s="3">
+        <v>946</v>
+      </c>
+      <c r="H6" s="3">
+        <v>6.31</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
+        <v>150</v>
+      </c>
+      <c r="D7" s="3">
+        <v>16</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.1067</v>
+      </c>
+      <c r="F7" s="3">
+        <v>150</v>
+      </c>
+      <c r="G7" s="3">
+        <v>670</v>
+      </c>
+      <c r="H7" s="3">
+        <v>4.47</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3">
+        <v>150</v>
+      </c>
+      <c r="D8" s="3">
+        <v>16</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.1067</v>
+      </c>
+      <c r="F8" s="3">
+        <v>150</v>
+      </c>
+      <c r="G8" s="3">
+        <v>660</v>
+      </c>
+      <c r="H8" s="28">
+        <v>4.4000000000000004</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3">
+        <v>150</v>
+      </c>
+      <c r="D9" s="3">
+        <v>18</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.12</v>
+      </c>
+      <c r="F9" s="3">
+        <v>150</v>
+      </c>
+      <c r="G9" s="3">
+        <v>402</v>
+      </c>
+      <c r="H9" s="3">
+        <v>2.68</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3">
+        <v>150</v>
+      </c>
+      <c r="D10" s="3">
+        <v>20</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.1333</v>
+      </c>
+      <c r="F10" s="3">
+        <v>150</v>
+      </c>
+      <c r="G10" s="3">
+        <v>504</v>
+      </c>
+      <c r="H10" s="3">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3">
+        <v>150</v>
+      </c>
+      <c r="D11" s="3">
+        <v>18</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.12</v>
+      </c>
+      <c r="F11" s="3">
+        <v>150</v>
+      </c>
+      <c r="G11" s="3">
+        <v>471</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3.14</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="46" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <v>150</v>
+      </c>
+      <c r="D12" s="3">
+        <v>25</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="F12" s="3">
+        <v>150</v>
+      </c>
+      <c r="G12" s="3">
+        <v>293</v>
+      </c>
+      <c r="H12" s="3">
+        <v>1.95</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3">
+        <v>150</v>
+      </c>
+      <c r="D13" s="3">
+        <v>17</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.1133</v>
+      </c>
+      <c r="F13" s="3">
+        <v>150</v>
+      </c>
+      <c r="G13" s="3">
+        <v>699</v>
+      </c>
+      <c r="H13" s="3">
+        <v>4.66</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3">
+        <v>150</v>
+      </c>
+      <c r="D14" s="3">
+        <v>19</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="F14" s="3">
+        <v>150</v>
+      </c>
+      <c r="G14" s="3">
+        <v>559</v>
+      </c>
+      <c r="H14" s="3">
+        <v>3.73</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C74F51-BDAD-924D-AEFA-68C8E4D340A8}">
+  <dimension ref="B2:H14"/>
+  <sheetViews>
+    <sheetView zoomScale="138" workbookViewId="0">
+      <selection activeCell="E16" sqref="E16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B2" s="3"/>
+      <c r="C2" s="15" t="s">
+        <v>4</v>
+      </c>
+      <c r="D2" s="15"/>
+      <c r="E2" s="15"/>
+      <c r="F2" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="G2" s="15"/>
+      <c r="H2" s="15"/>
+    </row>
+    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="G3" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="H3" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="3">
+        <v>100</v>
+      </c>
+      <c r="D4" s="3">
+        <v>3</v>
+      </c>
+      <c r="E4" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="F4" s="3">
+        <v>100</v>
+      </c>
+      <c r="G4" s="3">
+        <v>922</v>
+      </c>
+      <c r="H4" s="3">
+        <v>9.2200000000000006</v>
+      </c>
+    </row>
+    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>12</v>
+      </c>
+      <c r="C5" s="3">
+        <v>100</v>
+      </c>
+      <c r="D5" s="3">
+        <v>5</v>
+      </c>
+      <c r="E5" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="F5" s="3">
+        <v>100</v>
+      </c>
+      <c r="G5" s="3">
+        <v>688</v>
+      </c>
+      <c r="H5" s="3">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="C6" s="3">
+        <v>100</v>
+      </c>
+      <c r="D6" s="3">
+        <v>2</v>
+      </c>
+      <c r="E6" s="13">
+        <v>0.02</v>
+      </c>
+      <c r="F6" s="3">
+        <v>100</v>
+      </c>
+      <c r="G6" s="3">
+        <v>712</v>
+      </c>
+      <c r="H6" s="3">
+        <v>7.12</v>
+      </c>
+    </row>
+    <row r="7" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="C7" s="3">
+        <v>100</v>
+      </c>
+      <c r="D7" s="3">
+        <v>3</v>
+      </c>
+      <c r="E7" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="F7" s="3">
+        <v>100</v>
+      </c>
+      <c r="G7" s="3">
+        <v>693</v>
+      </c>
+      <c r="H7" s="3">
+        <v>6.93</v>
+      </c>
+    </row>
+    <row r="8" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C8" s="3">
+        <v>100</v>
+      </c>
+      <c r="D8" s="3">
+        <v>4</v>
+      </c>
+      <c r="E8" s="13">
+        <v>0.04</v>
+      </c>
+      <c r="F8" s="3">
+        <v>100</v>
+      </c>
+      <c r="G8" s="3">
+        <v>694</v>
+      </c>
+      <c r="H8" s="3">
+        <v>6.94</v>
+      </c>
+    </row>
+    <row r="9" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="3" t="s">
+        <v>19</v>
+      </c>
+      <c r="C9" s="3">
+        <v>100</v>
+      </c>
+      <c r="D9" s="3">
+        <v>5</v>
+      </c>
+      <c r="E9" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="F9" s="3">
+        <v>100</v>
+      </c>
+      <c r="G9" s="3">
+        <v>748</v>
+      </c>
+      <c r="H9" s="3">
+        <v>7.48</v>
+      </c>
+    </row>
+    <row r="10" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B10" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C10" s="3">
+        <v>100</v>
+      </c>
+      <c r="D10" s="3">
+        <v>3</v>
+      </c>
+      <c r="E10" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="F10" s="3">
+        <v>100</v>
+      </c>
+      <c r="G10" s="3">
+        <v>663</v>
+      </c>
+      <c r="H10" s="3">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" s="3">
+        <v>100</v>
+      </c>
+      <c r="D11" s="3">
+        <v>5</v>
+      </c>
+      <c r="E11" s="13">
+        <v>0.05</v>
+      </c>
+      <c r="F11" s="3">
+        <v>100</v>
+      </c>
+      <c r="G11" s="29">
+        <v>754</v>
+      </c>
+      <c r="H11" s="3">
+        <v>7.54</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C12" s="3">
+        <v>100</v>
+      </c>
+      <c r="D12" s="3">
+        <v>4</v>
+      </c>
+      <c r="E12" s="13">
+        <v>0.04</v>
+      </c>
+      <c r="F12" s="3">
+        <v>100</v>
+      </c>
+      <c r="G12" s="3">
+        <v>688</v>
+      </c>
+      <c r="H12" s="3">
+        <v>6.88</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C13" s="3">
+        <v>100</v>
+      </c>
+      <c r="D13" s="3">
+        <v>4</v>
+      </c>
+      <c r="E13" s="13">
+        <v>0.04</v>
+      </c>
+      <c r="F13" s="3">
+        <v>100</v>
+      </c>
+      <c r="G13" s="3">
+        <v>732</v>
+      </c>
+      <c r="H13" s="3">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C14" s="3">
+        <v>100</v>
+      </c>
+      <c r="D14" s="3">
+        <v>3</v>
+      </c>
+      <c r="E14" s="13">
+        <v>0.03</v>
+      </c>
+      <c r="F14" s="3">
+        <v>100</v>
+      </c>
+      <c r="G14" s="3">
+        <v>675</v>
+      </c>
+      <c r="H14" s="3">
+        <v>6.75</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="C2:E2"/>
+    <mergeCell ref="F2:H2"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15506EA-4930-9441-B4F3-EDD7A1FF6E26}">
+  <dimension ref="B2:F25"/>
+  <sheetViews>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="136" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="22.83203125" customWidth="1"/>
+    <col min="3" max="3" width="20.83203125" customWidth="1"/>
+    <col min="4" max="6" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B2" s="3"/>
+      <c r="C2" s="16" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="16"/>
+      <c r="E2" s="16"/>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B3" s="3"/>
+      <c r="C3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="D3" s="17" t="s">
+        <v>0</v>
+      </c>
+      <c r="E3" s="17" t="s">
+        <v>7</v>
+      </c>
+      <c r="F3" s="17" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B4" s="41" t="s">
+        <v>11</v>
+      </c>
+      <c r="C4" s="42" t="s">
+        <v>17</v>
+      </c>
+      <c r="D4" s="43">
+        <v>150</v>
+      </c>
+      <c r="E4" s="43">
+        <v>96</v>
+      </c>
+      <c r="F4" s="44">
+        <v>0.64</v>
+      </c>
+    </row>
+    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B5" s="45"/>
+      <c r="C5" s="42" t="s">
+        <v>16</v>
+      </c>
+      <c r="D5" s="43">
+        <v>100</v>
+      </c>
+      <c r="E5" s="43">
+        <v>71</v>
+      </c>
+      <c r="F5" s="44">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="18" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="19" t="s">
+        <v>17</v>
+      </c>
+      <c r="D6" s="20">
+        <v>150</v>
+      </c>
+      <c r="E6" s="20">
+        <v>107</v>
+      </c>
+      <c r="F6" s="21">
+        <v>0.71330000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="22"/>
+      <c r="C7" s="19" t="s">
+        <v>16</v>
+      </c>
+      <c r="D7" s="20">
+        <v>100</v>
+      </c>
+      <c r="E7" s="20">
+        <v>74</v>
+      </c>
+      <c r="F7" s="21">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="23" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="24" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" s="25">
+        <v>150</v>
+      </c>
+      <c r="E8" s="25">
+        <v>85</v>
+      </c>
+      <c r="F8" s="26">
+        <v>0.56659999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="27"/>
+      <c r="C9" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D9" s="25">
+        <v>100</v>
+      </c>
+      <c r="E9" s="25">
+        <v>71</v>
+      </c>
+      <c r="F9" s="26">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="31" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="32" t="s">
+        <v>17</v>
+      </c>
+      <c r="D10" s="33">
+        <v>150</v>
+      </c>
+      <c r="E10" s="33">
+        <v>102</v>
+      </c>
+      <c r="F10" s="34">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="35"/>
+      <c r="C11" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="D11" s="33">
+        <v>100</v>
+      </c>
+      <c r="E11" s="33">
+        <v>77</v>
+      </c>
+      <c r="F11" s="34">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="36" t="s">
+        <v>15</v>
+      </c>
+      <c r="C12" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D12" s="38">
+        <v>150</v>
+      </c>
+      <c r="E12" s="38">
+        <v>100</v>
+      </c>
+      <c r="F12" s="39">
+        <v>0.66669999999999996</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="40"/>
+      <c r="C13" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D13" s="38">
+        <v>100</v>
+      </c>
+      <c r="E13" s="38">
+        <v>76</v>
+      </c>
+      <c r="F13" s="39">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="36" t="s">
+        <v>19</v>
+      </c>
+      <c r="C14" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D14" s="38">
+        <v>150</v>
+      </c>
+      <c r="E14" s="38">
+        <v>97</v>
+      </c>
+      <c r="F14" s="39">
+        <v>0.64670000000000005</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="40"/>
+      <c r="C15" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D15" s="38">
+        <v>100</v>
+      </c>
+      <c r="E15" s="38">
+        <v>74</v>
+      </c>
+      <c r="F15" s="39">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="36" t="s">
+        <v>20</v>
+      </c>
+      <c r="C16" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D16" s="38">
+        <v>150</v>
+      </c>
+      <c r="E16" s="38">
+        <v>102</v>
+      </c>
+      <c r="F16" s="39">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="40"/>
+      <c r="C17" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D17" s="38">
+        <v>100</v>
+      </c>
+      <c r="E17" s="38">
+        <v>74</v>
+      </c>
+      <c r="F17" s="39">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="36" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" s="38">
+        <v>150</v>
+      </c>
+      <c r="E18" s="38">
+        <v>98</v>
+      </c>
+      <c r="F18" s="39">
+        <v>0.65329999999999999</v>
+      </c>
+    </row>
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="40"/>
+      <c r="C19" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D19" s="38">
+        <v>100</v>
+      </c>
+      <c r="E19" s="38">
+        <v>69</v>
+      </c>
+      <c r="F19" s="39">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="47" t="s">
+        <v>22</v>
+      </c>
+      <c r="C20" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D20" s="38">
+        <v>150</v>
+      </c>
+      <c r="E20" s="38">
+        <v>112</v>
+      </c>
+      <c r="F20" s="39">
+        <v>0.74670000000000003</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="48"/>
+      <c r="C21" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D21" s="38">
+        <v>100</v>
+      </c>
+      <c r="E21" s="38">
+        <v>75</v>
+      </c>
+      <c r="F21" s="39">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="47" t="s">
+        <v>23</v>
+      </c>
+      <c r="C22" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D22" s="38">
+        <v>150</v>
+      </c>
+      <c r="E22" s="38">
+        <v>116</v>
+      </c>
+      <c r="F22" s="39">
+        <v>0.77329999999999999</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="48"/>
+      <c r="C23" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D23" s="38">
+        <v>100</v>
+      </c>
+      <c r="E23" s="38">
+        <v>73</v>
+      </c>
+      <c r="F23" s="39">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="47" t="s">
+        <v>24</v>
+      </c>
+      <c r="C24" s="37" t="s">
+        <v>17</v>
+      </c>
+      <c r="D24" s="38">
+        <v>150</v>
+      </c>
+      <c r="E24" s="38">
+        <v>118</v>
+      </c>
+      <c r="F24" s="39">
+        <v>0.78669999999999995</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="48"/>
+      <c r="C25" s="37" t="s">
+        <v>16</v>
+      </c>
+      <c r="D25" s="38">
+        <v>100</v>
+      </c>
+      <c r="E25" s="38">
+        <v>77</v>
+      </c>
+      <c r="F25" s="39">
+        <v>0.77</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="12">
+    <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="B14:B15"/>
+    <mergeCell ref="B16:B17"/>
+    <mergeCell ref="B18:B19"/>
+    <mergeCell ref="B20:B21"/>
+    <mergeCell ref="B22:B23"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+  </mergeCells>
+  <phoneticPr fontId="3" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5945934-C971-AB47-BC34-D31B5F594263}">
+  <dimension ref="B1:E5"/>
+  <sheetViews>
+    <sheetView zoomScale="125" workbookViewId="0">
+      <selection activeCell="H11" sqref="H11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="20.83203125" customWidth="1"/>
+    <col min="3" max="5" width="12.83203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B2" s="1"/>
+      <c r="C2" s="10" t="s">
+        <v>8</v>
+      </c>
+      <c r="D2" s="11"/>
+      <c r="E2" s="12"/>
+    </row>
+    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B3" s="2"/>
+      <c r="C3" s="5" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="5" t="s">
+        <v>7</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
+      <c r="B4" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="C4" s="5">
+        <v>250</v>
+      </c>
+      <c r="D4" s="5">
+        <v>163</v>
+      </c>
+      <c r="E4" s="7">
+        <v>0.65200000000000002</v>
+      </c>
+    </row>
+    <row r="5" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B5" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C5" s="8">
+        <v>250</v>
+      </c>
+      <c r="D5" s="8">
+        <v>116</v>
+      </c>
+      <c r="E5" s="9">
+        <v>0.46400000000000002</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="C2:E2"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9F312D-430D-0042-B1CF-DB1A21B73BB7}">
   <dimension ref="B2:H5"/>
   <sheetViews>
@@ -1374,474 +2950,4 @@
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA613D23-B9DE-0542-95AA-364F896410C8}">
-  <dimension ref="B2:H6"/>
-  <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="H11" sqref="H11"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="8" width="12.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
-        <v>150</v>
-      </c>
-      <c r="D4" s="3">
-        <v>5</v>
-      </c>
-      <c r="E4" s="13">
-        <v>3.3300000000000003E-2</v>
-      </c>
-      <c r="F4" s="3">
-        <v>150</v>
-      </c>
-      <c r="G4" s="3">
-        <v>1640</v>
-      </c>
-      <c r="H4" s="3">
-        <v>10.93</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3">
-        <v>150</v>
-      </c>
-      <c r="D5" s="3">
-        <v>23</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0.15329999999999999</v>
-      </c>
-      <c r="F5" s="3">
-        <v>150</v>
-      </c>
-      <c r="G5" s="3">
-        <v>283</v>
-      </c>
-      <c r="H5" s="3">
-        <v>1.89</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3">
-        <v>150</v>
-      </c>
-      <c r="D6" s="3">
-        <v>9</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0.06</v>
-      </c>
-      <c r="F6" s="3">
-        <v>150</v>
-      </c>
-      <c r="G6" s="3">
-        <v>946</v>
-      </c>
-      <c r="H6" s="3">
-        <v>6.31</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C74F51-BDAD-924D-AEFA-68C8E4D340A8}">
-  <dimension ref="B2:H6"/>
-  <sheetViews>
-    <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="F17" sqref="F17:F18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="8" width="12.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
-        <v>4</v>
-      </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
-        <v>3</v>
-      </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
-    </row>
-    <row r="3" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="3" t="s">
-        <v>1</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>2</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>0</v>
-      </c>
-      <c r="G3" s="3" t="s">
-        <v>5</v>
-      </c>
-      <c r="H3" s="3" t="s">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="4" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B4" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="3">
-        <v>100</v>
-      </c>
-      <c r="D4" s="3">
-        <v>3</v>
-      </c>
-      <c r="E4" s="13">
-        <v>0.03</v>
-      </c>
-      <c r="F4" s="3">
-        <v>100</v>
-      </c>
-      <c r="G4" s="3">
-        <v>922</v>
-      </c>
-      <c r="H4" s="3">
-        <v>9.2200000000000006</v>
-      </c>
-    </row>
-    <row r="5" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="C5" s="3">
-        <v>100</v>
-      </c>
-      <c r="D5" s="3">
-        <v>5</v>
-      </c>
-      <c r="E5" s="13">
-        <v>0.05</v>
-      </c>
-      <c r="F5" s="3">
-        <v>100</v>
-      </c>
-      <c r="G5" s="3">
-        <v>688</v>
-      </c>
-      <c r="H5" s="3">
-        <v>6.88</v>
-      </c>
-    </row>
-    <row r="6" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="3" t="s">
-        <v>13</v>
-      </c>
-      <c r="C6" s="3">
-        <v>100</v>
-      </c>
-      <c r="D6" s="3">
-        <v>2</v>
-      </c>
-      <c r="E6" s="13">
-        <v>0.02</v>
-      </c>
-      <c r="F6" s="3">
-        <v>100</v>
-      </c>
-      <c r="G6" s="3">
-        <v>712</v>
-      </c>
-      <c r="H6" s="3">
-        <v>7.12</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="2">
-    <mergeCell ref="C2:E2"/>
-    <mergeCell ref="F2:H2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{C5945934-C971-AB47-BC34-D31B5F594263}">
-  <dimension ref="B1:E5"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:E5"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="2" width="20.83203125" customWidth="1"/>
-    <col min="3" max="5" width="12.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="2" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B2" s="1"/>
-      <c r="C2" s="10" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
-    </row>
-    <row r="3" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B3" s="2"/>
-      <c r="C3" s="5" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="5" t="s">
-        <v>7</v>
-      </c>
-      <c r="E3" s="6" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
-      <c r="B4" s="2" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" s="5">
-        <v>250</v>
-      </c>
-      <c r="D4" s="5">
-        <v>163</v>
-      </c>
-      <c r="E4" s="7">
-        <v>0.65200000000000002</v>
-      </c>
-    </row>
-    <row r="5" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B5" s="4" t="s">
-        <v>10</v>
-      </c>
-      <c r="C5" s="8">
-        <v>250</v>
-      </c>
-      <c r="D5" s="8">
-        <v>116</v>
-      </c>
-      <c r="E5" s="9">
-        <v>0.46400000000000002</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="1">
-    <mergeCell ref="C2:E2"/>
-  </mergeCells>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
-</file>
-
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15506EA-4930-9441-B4F3-EDD7A1FF6E26}">
-  <dimension ref="B2:F9"/>
-  <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E17" sqref="E17:E18"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="2" max="3" width="20.83203125" customWidth="1"/>
-    <col min="4" max="6" width="12.83203125" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="2" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B2" s="3"/>
-      <c r="C2" s="16" t="s">
-        <v>8</v>
-      </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B3" s="3"/>
-      <c r="C3" s="3" t="s">
-        <v>16</v>
-      </c>
-      <c r="D3" s="17" t="s">
-        <v>0</v>
-      </c>
-      <c r="E3" s="17" t="s">
-        <v>7</v>
-      </c>
-      <c r="F3" s="17" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="18" t="s">
-        <v>11</v>
-      </c>
-      <c r="C4" s="19" t="s">
-        <v>15</v>
-      </c>
-      <c r="D4" s="20">
-        <v>150</v>
-      </c>
-      <c r="E4" s="20">
-        <v>96</v>
-      </c>
-      <c r="F4" s="21">
-        <v>0.64</v>
-      </c>
-    </row>
-    <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="22"/>
-      <c r="C5" s="19" t="s">
-        <v>14</v>
-      </c>
-      <c r="D5" s="20">
-        <v>100</v>
-      </c>
-      <c r="E5" s="20">
-        <v>71</v>
-      </c>
-      <c r="F5" s="21">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="23" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="24" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6" s="25">
-        <v>150</v>
-      </c>
-      <c r="E6" s="25">
-        <v>107</v>
-      </c>
-      <c r="F6" s="26">
-        <v>0.71330000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="27"/>
-      <c r="C7" s="24" t="s">
-        <v>14</v>
-      </c>
-      <c r="D7" s="25">
-        <v>100</v>
-      </c>
-      <c r="E7" s="25">
-        <v>74</v>
-      </c>
-      <c r="F7" s="26">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="28" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="29" t="s">
-        <v>15</v>
-      </c>
-      <c r="D8" s="30">
-        <v>150</v>
-      </c>
-      <c r="E8" s="30">
-        <v>85</v>
-      </c>
-      <c r="F8" s="31">
-        <v>0.56659999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="32"/>
-      <c r="C9" s="29" t="s">
-        <v>14</v>
-      </c>
-      <c r="D9" s="30">
-        <v>100</v>
-      </c>
-      <c r="E9" s="30">
-        <v>71</v>
-      </c>
-      <c r="F9" s="31">
-        <v>0.71</v>
-      </c>
-    </row>
-  </sheetData>
-  <mergeCells count="4">
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-  </mergeCells>
-  <phoneticPr fontId="2" type="noConversion"/>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
prompt v4 baseline eval
</commit_message>
<xml_diff>
--- a/evaluation/results_by_data_split.xlsx
+++ b/evaluation/results_by_data_split.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yufeizhao/Desktop/11667MiniProject/11667-NLP2SQL/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2DA5B968-A8F9-A34A-91E4-545B63CD127D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F569FA4-FB7C-F14E-9508-7A16899B31A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1700" yWindow="-20560" windowWidth="28040" windowHeight="17440" activeTab="5" xr2:uid="{44081516-0D10-9B41-9157-44A5B55A14F9}"/>
+    <workbookView xWindow="-1700" yWindow="-20560" windowWidth="28040" windowHeight="19460" activeTab="5" xr2:uid="{44081516-0D10-9B41-9157-44A5B55A14F9}"/>
   </bookViews>
   <sheets>
     <sheet name="train_sql2sql" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="147" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="30">
   <si>
     <t>total queries</t>
   </si>
@@ -90,9 +90,6 @@
     <t>promptv3_codellama_v6</t>
   </si>
   <si>
-    <t>promptv3_codellama_v7</t>
-  </si>
-  <si>
     <t>eval_test</t>
   </si>
   <si>
@@ -102,22 +99,40 @@
     <t>data_split</t>
   </si>
   <si>
-    <t>promptv3_codellama_v7.1</t>
+    <t>promptv3_deepseek_v0</t>
   </si>
   <si>
-    <t>promptv3_codellama_v7.2</t>
+    <t>promptv3_sqlcoder_v0</t>
   </si>
   <si>
-    <t>promptv3_codellama_v7.3</t>
+    <t>promptv4_codellama_v7</t>
   </si>
   <si>
-    <t>promptv3_codellama_v7.4</t>
+    <t>promptv4_codellama_v7.1</t>
   </si>
   <si>
-    <t>promptv3_codellama_v7.5</t>
+    <t>promptv4_codellama_v7.2</t>
   </si>
   <si>
-    <t>promptv3_codellama_v7.6</t>
+    <t>promptv4_codellama_v7.3</t>
+  </si>
+  <si>
+    <t>promptv4_codellama_v7.4</t>
+  </si>
+  <si>
+    <t>promptv4_codellama_v7.5</t>
+  </si>
+  <si>
+    <t>promptv4_codellama_v7.6</t>
+  </si>
+  <si>
+    <t>promptv4_deepseek_v0</t>
+  </si>
+  <si>
+    <t>promptv4_sqlcoder_v0</t>
+  </si>
+  <si>
+    <t>promptv4_codellama_v0</t>
   </si>
 </sst>
 </file>
@@ -153,7 +168,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="7">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -190,6 +205,18 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC3C3F2"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFF8F5C3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
   <borders count="15">
     <border>
@@ -381,7 +408,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="49">
+  <cellXfs count="60">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -410,6 +437,111 @@
     <xf numFmtId="10" fontId="1" fillId="0" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -419,112 +551,40 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="4" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="5" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -533,6 +593,12 @@
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <mruColors>
+      <color rgb="FFF8F5C3"/>
+      <color rgb="FFC3C3F2"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -875,16 +941,16 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -917,7 +983,7 @@
       <c r="D4" s="3">
         <v>358</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>0.2387</v>
       </c>
       <c r="F4" s="3">
@@ -940,7 +1006,7 @@
       <c r="D5" s="3">
         <v>903</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>0.60199999999999998</v>
       </c>
       <c r="F5" s="3">
@@ -963,7 +1029,7 @@
       <c r="D6" s="3">
         <v>402</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>0.24360000000000001</v>
       </c>
       <c r="F6" s="3">
@@ -977,16 +1043,16 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
-      <c r="C7" s="14">
+      <c r="C7" s="3">
         <v>1650</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="3">
         <v>1099</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>0.66610000000000003</v>
       </c>
       <c r="F7" s="3">
@@ -1000,7 +1066,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="3">
@@ -1009,7 +1075,7 @@
       <c r="D8" s="3">
         <v>980</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>0.59389999999999998</v>
       </c>
       <c r="F8" s="3">
@@ -1033,10 +1099,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C775F-3A5B-8346-B68B-D75012605A96}">
-  <dimension ref="B2:H16"/>
+  <dimension ref="B2:H19"/>
   <sheetViews>
     <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="H10" sqref="H10:H16"/>
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1047,16 +1113,16 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -1089,7 +1155,7 @@
       <c r="D4" s="3">
         <v>59</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>0.23599999999999999</v>
       </c>
       <c r="F4" s="3">
@@ -1112,7 +1178,7 @@
       <c r="D5" s="3">
         <v>128</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>0.51200000000000001</v>
       </c>
       <c r="F5" s="3">
@@ -1135,7 +1201,7 @@
       <c r="D6" s="3">
         <v>64</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>0.25600000000000001</v>
       </c>
       <c r="F6" s="3">
@@ -1149,16 +1215,16 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="3">
         <v>250</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="3">
         <v>138</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>0.55200000000000005</v>
       </c>
       <c r="F7" s="3">
@@ -1172,7 +1238,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="3">
@@ -1181,7 +1247,7 @@
       <c r="D8" s="3">
         <v>142</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>0.56799999999999995</v>
       </c>
       <c r="F8" s="3">
@@ -1195,7 +1261,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3">
@@ -1204,7 +1270,7 @@
       <c r="D9" s="3">
         <v>118</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <v>0.47199999999999998</v>
       </c>
       <c r="F9" s="3">
@@ -1218,164 +1284,233 @@
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="14" t="s">
-        <v>15</v>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="3">
         <v>250</v>
       </c>
       <c r="D10" s="3">
+        <v>68</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="F10" s="3">
+        <v>250</v>
+      </c>
+      <c r="G10" s="3">
+        <v>1729</v>
+      </c>
+      <c r="H10" s="3">
+        <v>6.92</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>250</v>
+      </c>
+      <c r="D11" s="3">
         <v>116</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E11" s="10">
         <v>0.46400000000000002</v>
       </c>
-      <c r="F10" s="3">
-        <v>250</v>
-      </c>
-      <c r="G10" s="3">
+      <c r="F11" s="3">
+        <v>250</v>
+      </c>
+      <c r="G11" s="3">
         <v>862</v>
       </c>
-      <c r="H10" s="3">
+      <c r="H11" s="3">
         <v>3.45</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="14" t="s">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3">
+        <v>250</v>
+      </c>
+      <c r="D12" s="3">
+        <v>124</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.496</v>
+      </c>
+      <c r="F12" s="3">
+        <v>250</v>
+      </c>
+      <c r="G12" s="3">
+        <v>838</v>
+      </c>
+      <c r="H12" s="3">
+        <v>3.35</v>
+      </c>
+    </row>
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3">
+        <v>250</v>
+      </c>
+      <c r="D13" s="3">
+        <v>126</v>
+      </c>
+      <c r="E13" s="10">
+        <v>0.504</v>
+      </c>
+      <c r="F13" s="3">
+        <v>250</v>
+      </c>
+      <c r="G13" s="3">
+        <v>869</v>
+      </c>
+      <c r="H13" s="3">
+        <v>3.48</v>
+      </c>
+    </row>
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3">
+        <v>250</v>
+      </c>
+      <c r="D14" s="3">
+        <v>123</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="F14" s="3">
+        <v>250</v>
+      </c>
+      <c r="G14" s="3">
+        <v>850</v>
+      </c>
+      <c r="H14" s="18">
+        <v>3.4</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3">
+        <v>250</v>
+      </c>
+      <c r="D15" s="3">
+        <v>124</v>
+      </c>
+      <c r="E15" s="10">
+        <v>0.496</v>
+      </c>
+      <c r="F15" s="3">
+        <v>250</v>
+      </c>
+      <c r="G15" s="3">
+        <v>844</v>
+      </c>
+      <c r="H15" s="3">
+        <v>3.38</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3">
+        <v>250</v>
+      </c>
+      <c r="D16" s="3">
+        <v>108</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.432</v>
+      </c>
+      <c r="F16" s="3">
+        <v>250</v>
+      </c>
+      <c r="G16" s="3">
+        <v>966</v>
+      </c>
+      <c r="H16" s="3">
+        <v>3.86</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3">
+        <v>250</v>
+      </c>
+      <c r="D17" s="3">
+        <v>109</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.436</v>
+      </c>
+      <c r="F17" s="3">
+        <v>250</v>
+      </c>
+      <c r="G17" s="3">
+        <v>967</v>
+      </c>
+      <c r="H17" s="3">
+        <v>3.87</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C18" s="3">
+        <v>250</v>
+      </c>
+      <c r="D18" s="3">
+        <v>55</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="F18" s="3">
+        <v>250</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1657</v>
+      </c>
+      <c r="H18" s="3">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C11" s="3">
-        <v>250</v>
-      </c>
-      <c r="D11" s="3">
-        <v>124</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0.496</v>
-      </c>
-      <c r="F11" s="3">
-        <v>250</v>
-      </c>
-      <c r="G11" s="3">
-        <v>838</v>
-      </c>
-      <c r="H11" s="3">
-        <v>3.35</v>
-      </c>
-    </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3">
-        <v>250</v>
-      </c>
-      <c r="D12" s="3">
-        <v>126</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0.504</v>
-      </c>
-      <c r="F12" s="3">
-        <v>250</v>
-      </c>
-      <c r="G12" s="3">
-        <v>869</v>
-      </c>
-      <c r="H12" s="3">
-        <v>3.48</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3">
-        <v>250</v>
-      </c>
-      <c r="D13" s="3">
-        <v>123</v>
-      </c>
-      <c r="E13" s="13">
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="F13" s="3">
-        <v>250</v>
-      </c>
-      <c r="G13" s="3">
-        <v>850</v>
-      </c>
-      <c r="H13" s="28">
-        <v>3.4</v>
-      </c>
-    </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3">
-        <v>250</v>
-      </c>
-      <c r="D14" s="3">
-        <v>124</v>
-      </c>
-      <c r="E14" s="13">
-        <v>0.496</v>
-      </c>
-      <c r="F14" s="3">
-        <v>250</v>
-      </c>
-      <c r="G14" s="3">
-        <v>844</v>
-      </c>
-      <c r="H14" s="3">
-        <v>3.38</v>
-      </c>
-    </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="3">
-        <v>250</v>
-      </c>
-      <c r="D15" s="3">
-        <v>108</v>
-      </c>
-      <c r="E15" s="13">
-        <v>0.432</v>
-      </c>
-      <c r="F15" s="3">
-        <v>250</v>
-      </c>
-      <c r="G15" s="3">
-        <v>966</v>
-      </c>
-      <c r="H15" s="3">
-        <v>3.86</v>
-      </c>
-    </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="3">
-        <v>250</v>
-      </c>
-      <c r="D16" s="3">
-        <v>109</v>
-      </c>
-      <c r="E16" s="13">
-        <v>0.436</v>
-      </c>
-      <c r="F16" s="3">
-        <v>250</v>
-      </c>
-      <c r="G16" s="3">
-        <v>967</v>
-      </c>
-      <c r="H16" s="3">
-        <v>3.87</v>
+      <c r="C19" s="3">
+        <v>250</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="10">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F19" s="3">
+        <v>250</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2292</v>
+      </c>
+      <c r="H19" s="3">
+        <v>9.17</v>
       </c>
     </row>
   </sheetData>
@@ -1390,10 +1525,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82A48FE-26B2-E846-83D1-3D5B61BC4083}">
-  <dimension ref="B2:H16"/>
+  <dimension ref="B2:H20"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="F20" sqref="F20"/>
+      <selection activeCell="I9" sqref="I9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1404,16 +1539,16 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -1446,7 +1581,7 @@
       <c r="D4" s="3">
         <v>62</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>0.248</v>
       </c>
       <c r="F4" s="3">
@@ -1469,7 +1604,7 @@
       <c r="D5" s="3">
         <v>143</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>0.57199999999999995</v>
       </c>
       <c r="F5" s="3">
@@ -1492,7 +1627,7 @@
       <c r="D6" s="3">
         <v>68</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>0.27500000000000002</v>
       </c>
       <c r="F6" s="3">
@@ -1506,16 +1641,16 @@
       </c>
     </row>
     <row r="7" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="14" t="s">
+      <c r="B7" s="3" t="s">
         <v>12</v>
       </c>
       <c r="C7" s="3">
         <v>250</v>
       </c>
-      <c r="D7" s="14">
+      <c r="D7" s="3">
         <v>146</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>0.58399999999999996</v>
       </c>
       <c r="F7" s="3">
@@ -1529,7 +1664,7 @@
       </c>
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="14" t="s">
+      <c r="B8" s="3" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="3">
@@ -1538,7 +1673,7 @@
       <c r="D8" s="3">
         <v>147</v>
       </c>
-      <c r="E8" s="13">
+      <c r="E8" s="10">
         <v>0.58799999999999997</v>
       </c>
       <c r="F8" s="3">
@@ -1552,7 +1687,7 @@
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="14" t="s">
+      <c r="B9" s="3" t="s">
         <v>14</v>
       </c>
       <c r="C9" s="3">
@@ -1561,7 +1696,7 @@
       <c r="D9" s="3">
         <v>121</v>
       </c>
-      <c r="E9" s="13">
+      <c r="E9" s="10">
         <v>0.48399999999999999</v>
       </c>
       <c r="F9" s="3">
@@ -1570,170 +1705,243 @@
       <c r="G9" s="3">
         <v>925</v>
       </c>
-      <c r="H9" s="28">
+      <c r="H9" s="18">
         <v>3.7</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B10" s="14" t="s">
-        <v>15</v>
+      <c r="B10" s="3" t="s">
+        <v>29</v>
       </c>
       <c r="C10" s="3">
         <v>250</v>
       </c>
       <c r="D10" s="3">
+        <v>68</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.27200000000000002</v>
+      </c>
+      <c r="F10" s="3">
+        <v>250</v>
+      </c>
+      <c r="G10" s="19">
+        <v>1903</v>
+      </c>
+      <c r="H10" s="48">
+        <v>7.61</v>
+      </c>
+    </row>
+    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="3" t="s">
+        <v>20</v>
+      </c>
+      <c r="C11" s="3">
+        <v>250</v>
+      </c>
+      <c r="D11" s="3">
         <v>127</v>
       </c>
-      <c r="E10" s="13">
+      <c r="E11" s="10">
         <v>0.50800000000000001</v>
       </c>
-      <c r="F10" s="3">
-        <v>250</v>
-      </c>
-      <c r="G10" s="29">
+      <c r="F11" s="3">
+        <v>250</v>
+      </c>
+      <c r="G11" s="19">
         <v>890</v>
       </c>
-      <c r="H10" s="29">
+      <c r="H11" s="19">
         <v>3.56</v>
       </c>
     </row>
-    <row r="11" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="14" t="s">
-        <v>19</v>
-      </c>
-      <c r="C11" s="3">
-        <v>250</v>
-      </c>
-      <c r="D11" s="3">
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" s="3">
+        <v>250</v>
+      </c>
+      <c r="D12" s="3">
         <v>124</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E12" s="10">
         <v>0.496</v>
       </c>
-      <c r="F11" s="3">
-        <v>250</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="F12" s="3">
+        <v>250</v>
+      </c>
+      <c r="G12" s="3">
         <v>899</v>
       </c>
-      <c r="H11" s="28">
+      <c r="H12" s="18">
         <v>3.6</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="14" t="s">
-        <v>20</v>
-      </c>
-      <c r="C12" s="3">
-        <v>250</v>
-      </c>
-      <c r="D12" s="3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>22</v>
+      </c>
+      <c r="C13" s="3">
+        <v>250</v>
+      </c>
+      <c r="D13" s="3">
         <v>132</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E13" s="10">
         <v>0.52800000000000002</v>
       </c>
-      <c r="F12" s="3">
-        <v>250</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F13" s="3">
+        <v>250</v>
+      </c>
+      <c r="G13" s="3">
         <v>869</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H13" s="3">
         <v>3.48</v>
       </c>
     </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="14" t="s">
-        <v>21</v>
-      </c>
-      <c r="C13" s="3">
-        <v>250</v>
-      </c>
-      <c r="D13" s="3">
+    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C14" s="3">
+        <v>250</v>
+      </c>
+      <c r="D14" s="3">
         <v>125</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E14" s="10">
         <v>0.5</v>
       </c>
-      <c r="F13" s="3">
-        <v>250</v>
-      </c>
-      <c r="G13" s="3">
+      <c r="F14" s="3">
+        <v>250</v>
+      </c>
+      <c r="G14" s="3">
         <v>876</v>
       </c>
-      <c r="H13" s="28">
+      <c r="H14" s="18">
         <v>3.5</v>
       </c>
     </row>
-    <row r="14" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="14" t="s">
-        <v>22</v>
-      </c>
-      <c r="C14" s="3">
-        <v>250</v>
-      </c>
-      <c r="D14" s="3">
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="C15" s="3">
+        <v>250</v>
+      </c>
+      <c r="D15" s="3">
         <v>138</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E15" s="10">
         <v>0.55200000000000005</v>
       </c>
-      <c r="F14" s="3">
-        <v>250</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F15" s="3">
+        <v>250</v>
+      </c>
+      <c r="G15" s="3">
         <v>840</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="3">
         <v>3.36</v>
       </c>
     </row>
-    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="14" t="s">
-        <v>23</v>
-      </c>
-      <c r="C15" s="3">
-        <v>250</v>
-      </c>
-      <c r="D15" s="29">
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C16" s="3">
+        <v>250</v>
+      </c>
+      <c r="D16" s="19">
         <v>125</v>
       </c>
-      <c r="E15" s="30">
+      <c r="E16" s="20">
         <v>0.5</v>
       </c>
-      <c r="F15" s="3">
-        <v>250</v>
-      </c>
-      <c r="G15" s="3">
+      <c r="F16" s="3">
+        <v>250</v>
+      </c>
+      <c r="G16" s="3">
         <v>935</v>
       </c>
-      <c r="H15" s="3">
+      <c r="H16" s="3">
         <v>3.74</v>
       </c>
     </row>
-    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="14" t="s">
-        <v>24</v>
-      </c>
-      <c r="C16" s="3">
-        <v>250</v>
-      </c>
-      <c r="D16" s="3">
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C17" s="3">
+        <v>250</v>
+      </c>
+      <c r="D17" s="3">
         <v>125</v>
       </c>
-      <c r="E16" s="13">
+      <c r="E17" s="10">
         <v>0.5</v>
       </c>
-      <c r="F16" s="3">
-        <v>250</v>
-      </c>
-      <c r="G16" s="3">
+      <c r="F17" s="3">
+        <v>250</v>
+      </c>
+      <c r="G17" s="3">
         <v>912</v>
       </c>
-      <c r="H16" s="3">
+      <c r="H17" s="3">
         <v>3.65</v>
       </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C18" s="3">
+        <v>250</v>
+      </c>
+      <c r="D18" s="3">
+        <v>58</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="F18" s="3">
+        <v>250</v>
+      </c>
+      <c r="G18" s="3">
+        <v>1677</v>
+      </c>
+      <c r="H18" s="3">
+        <v>6.71</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C19" s="3">
+        <v>250</v>
+      </c>
+      <c r="D19" s="3">
+        <v>2</v>
+      </c>
+      <c r="E19" s="10">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F19" s="3">
+        <v>250</v>
+      </c>
+      <c r="G19" s="3">
+        <v>2273</v>
+      </c>
+      <c r="H19" s="3">
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="D20" s="49"/>
+      <c r="E20" s="49"/>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -1747,30 +1955,30 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA613D23-B9DE-0542-95AA-364F896410C8}">
-  <dimension ref="B2:H14"/>
+  <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="I18" sqref="I18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="8" width="12.83203125" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" style="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -1803,7 +2011,7 @@
       <c r="D4" s="3">
         <v>5</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>3.3300000000000003E-2</v>
       </c>
       <c r="F4" s="3">
@@ -1826,7 +2034,7 @@
       <c r="D5" s="3">
         <v>23</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>0.15329999999999999</v>
       </c>
       <c r="F5" s="3">
@@ -1849,7 +2057,7 @@
       <c r="D6" s="3">
         <v>9</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>0.06</v>
       </c>
       <c r="F6" s="3">
@@ -1872,7 +2080,7 @@
       <c r="D7" s="3">
         <v>16</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>0.1067</v>
       </c>
       <c r="F7" s="3">
@@ -1887,163 +2095,232 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3">
         <v>150</v>
       </c>
       <c r="D8" s="3">
-        <v>16</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0.1067</v>
+        <v>5</v>
+      </c>
+      <c r="E8" s="10">
+        <v>3.3300000000000003E-2</v>
       </c>
       <c r="F8" s="3">
         <v>150</v>
       </c>
       <c r="G8" s="3">
-        <v>660</v>
-      </c>
-      <c r="H8" s="28">
-        <v>4.4000000000000004</v>
+        <v>2030</v>
+      </c>
+      <c r="H8" s="3">
+        <v>13.53</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>150</v>
       </c>
       <c r="D9" s="3">
-        <v>18</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0.12</v>
+        <v>16</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.1067</v>
       </c>
       <c r="F9" s="3">
         <v>150</v>
       </c>
       <c r="G9" s="3">
-        <v>402</v>
-      </c>
-      <c r="H9" s="3">
-        <v>2.68</v>
+        <v>660</v>
+      </c>
+      <c r="H9" s="18">
+        <v>4.4000000000000004</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
         <v>150</v>
       </c>
       <c r="D10" s="3">
-        <v>20</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0.1333</v>
+        <v>18</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.12</v>
       </c>
       <c r="F10" s="3">
         <v>150</v>
       </c>
       <c r="G10" s="3">
-        <v>504</v>
+        <v>402</v>
       </c>
       <c r="H10" s="3">
-        <v>3.36</v>
+        <v>2.68</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>150</v>
       </c>
       <c r="D11" s="3">
+        <v>20</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.1333</v>
+      </c>
+      <c r="F11" s="3">
+        <v>150</v>
+      </c>
+      <c r="G11" s="3">
+        <v>504</v>
+      </c>
+      <c r="H11" s="3">
+        <v>3.36</v>
+      </c>
+    </row>
+    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="3" t="s">
+        <v>23</v>
+      </c>
+      <c r="C12" s="3">
+        <v>150</v>
+      </c>
+      <c r="D12" s="3">
         <v>18</v>
       </c>
-      <c r="E11" s="13">
+      <c r="E12" s="10">
         <v>0.12</v>
       </c>
-      <c r="F11" s="3">
-        <v>150</v>
-      </c>
-      <c r="G11" s="3">
+      <c r="F12" s="3">
+        <v>150</v>
+      </c>
+      <c r="G12" s="3">
         <v>471</v>
       </c>
-      <c r="H11" s="3">
+      <c r="H12" s="3">
         <v>3.14</v>
       </c>
     </row>
-    <row r="12" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="46" t="s">
-        <v>22</v>
-      </c>
-      <c r="C12" s="3">
-        <v>150</v>
-      </c>
-      <c r="D12" s="3">
+    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="30" t="s">
+        <v>24</v>
+      </c>
+      <c r="C13" s="3">
+        <v>150</v>
+      </c>
+      <c r="D13" s="3">
         <v>25</v>
       </c>
-      <c r="E12" s="13">
+      <c r="E13" s="10">
         <v>0.16669999999999999</v>
       </c>
-      <c r="F12" s="3">
-        <v>150</v>
-      </c>
-      <c r="G12" s="3">
+      <c r="F13" s="3">
+        <v>150</v>
+      </c>
+      <c r="G13" s="3">
         <v>293</v>
       </c>
-      <c r="H12" s="3">
+      <c r="H13" s="3">
         <v>1.95</v>
-      </c>
-    </row>
-    <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="C13" s="3">
-        <v>150</v>
-      </c>
-      <c r="D13" s="3">
-        <v>17</v>
-      </c>
-      <c r="E13" s="13">
-        <v>0.1133</v>
-      </c>
-      <c r="F13" s="3">
-        <v>150</v>
-      </c>
-      <c r="G13" s="3">
-        <v>699</v>
-      </c>
-      <c r="H13" s="3">
-        <v>4.66</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3">
         <v>150</v>
       </c>
       <c r="D14" s="3">
+        <v>17</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.1133</v>
+      </c>
+      <c r="F14" s="3">
+        <v>150</v>
+      </c>
+      <c r="G14" s="3">
+        <v>699</v>
+      </c>
+      <c r="H14" s="3">
+        <v>4.66</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3">
+        <v>150</v>
+      </c>
+      <c r="D15" s="3">
         <v>19</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E15" s="10">
         <v>0.12670000000000001</v>
       </c>
-      <c r="F14" s="3">
-        <v>150</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F15" s="3">
+        <v>150</v>
+      </c>
+      <c r="G15" s="3">
         <v>559</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="3">
         <v>3.73</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3">
+        <v>150</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="F16" s="3">
+        <v>150</v>
+      </c>
+      <c r="G16" s="3">
+        <v>1605</v>
+      </c>
+      <c r="H16" s="3">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3">
+        <v>150</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>150</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1728</v>
+      </c>
+      <c r="H17" s="3">
+        <v>11.52</v>
       </c>
     </row>
   </sheetData>
@@ -2058,30 +2335,30 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C74F51-BDAD-924D-AEFA-68C8E4D340A8}">
-  <dimension ref="B2:H14"/>
+  <dimension ref="B2:H17"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="E16" sqref="E16"/>
+      <selection activeCell="E24" sqref="E24"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="8" width="12.83203125" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" style="49" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -2114,7 +2391,7 @@
       <c r="D4" s="3">
         <v>3</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>0.03</v>
       </c>
       <c r="F4" s="3">
@@ -2137,7 +2414,7 @@
       <c r="D5" s="3">
         <v>5</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>0.05</v>
       </c>
       <c r="F5" s="3">
@@ -2160,7 +2437,7 @@
       <c r="D6" s="3">
         <v>2</v>
       </c>
-      <c r="E6" s="13">
+      <c r="E6" s="10">
         <v>0.02</v>
       </c>
       <c r="F6" s="3">
@@ -2183,7 +2460,7 @@
       <c r="D7" s="3">
         <v>3</v>
       </c>
-      <c r="E7" s="13">
+      <c r="E7" s="10">
         <v>0.03</v>
       </c>
       <c r="F7" s="3">
@@ -2198,122 +2475,122 @@
     </row>
     <row r="8" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B8" s="3" t="s">
-        <v>15</v>
+        <v>29</v>
       </c>
       <c r="C8" s="3">
         <v>100</v>
       </c>
       <c r="D8" s="3">
-        <v>4</v>
-      </c>
-      <c r="E8" s="13">
-        <v>0.04</v>
+        <v>2</v>
+      </c>
+      <c r="E8" s="10">
+        <v>0.02</v>
       </c>
       <c r="F8" s="3">
         <v>100</v>
       </c>
       <c r="G8" s="3">
-        <v>694</v>
+        <v>1088</v>
       </c>
       <c r="H8" s="3">
-        <v>6.94</v>
+        <v>10.88</v>
       </c>
     </row>
     <row r="9" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B9" s="3" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C9" s="3">
         <v>100</v>
       </c>
       <c r="D9" s="3">
-        <v>5</v>
-      </c>
-      <c r="E9" s="13">
-        <v>0.05</v>
+        <v>4</v>
+      </c>
+      <c r="E9" s="10">
+        <v>0.04</v>
       </c>
       <c r="F9" s="3">
         <v>100</v>
       </c>
       <c r="G9" s="3">
-        <v>748</v>
+        <v>694</v>
       </c>
       <c r="H9" s="3">
-        <v>7.48</v>
+        <v>6.94</v>
       </c>
     </row>
     <row r="10" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B10" s="3" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="C10" s="3">
         <v>100</v>
       </c>
       <c r="D10" s="3">
-        <v>3</v>
-      </c>
-      <c r="E10" s="13">
-        <v>0.03</v>
+        <v>5</v>
+      </c>
+      <c r="E10" s="10">
+        <v>0.05</v>
       </c>
       <c r="F10" s="3">
         <v>100</v>
       </c>
       <c r="G10" s="3">
-        <v>663</v>
+        <v>748</v>
       </c>
       <c r="H10" s="3">
-        <v>6.63</v>
+        <v>7.48</v>
       </c>
     </row>
     <row r="11" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B11" s="3" t="s">
-        <v>21</v>
+        <v>22</v>
       </c>
       <c r="C11" s="3">
         <v>100</v>
       </c>
       <c r="D11" s="3">
-        <v>5</v>
-      </c>
-      <c r="E11" s="13">
-        <v>0.05</v>
+        <v>3</v>
+      </c>
+      <c r="E11" s="10">
+        <v>0.03</v>
       </c>
       <c r="F11" s="3">
         <v>100</v>
       </c>
-      <c r="G11" s="29">
-        <v>754</v>
+      <c r="G11" s="3">
+        <v>663</v>
       </c>
       <c r="H11" s="3">
-        <v>7.54</v>
+        <v>6.63</v>
       </c>
     </row>
     <row r="12" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B12" s="3" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="C12" s="3">
         <v>100</v>
       </c>
       <c r="D12" s="3">
-        <v>4</v>
-      </c>
-      <c r="E12" s="13">
-        <v>0.04</v>
+        <v>5</v>
+      </c>
+      <c r="E12" s="10">
+        <v>0.05</v>
       </c>
       <c r="F12" s="3">
         <v>100</v>
       </c>
       <c r="G12" s="3">
-        <v>688</v>
+        <v>754</v>
       </c>
       <c r="H12" s="3">
-        <v>6.88</v>
+        <v>7.54</v>
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="3" t="s">
-        <v>23</v>
+      <c r="B13" s="30" t="s">
+        <v>24</v>
       </c>
       <c r="C13" s="3">
         <v>100</v>
@@ -2321,40 +2598,109 @@
       <c r="D13" s="3">
         <v>4</v>
       </c>
-      <c r="E13" s="13">
+      <c r="E13" s="10">
         <v>0.04</v>
       </c>
       <c r="F13" s="3">
         <v>100</v>
       </c>
       <c r="G13" s="3">
-        <v>732</v>
+        <v>688</v>
       </c>
       <c r="H13" s="3">
-        <v>7.32</v>
+        <v>6.88</v>
       </c>
     </row>
     <row r="14" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B14" s="3" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="C14" s="3">
         <v>100</v>
       </c>
       <c r="D14" s="3">
+        <v>4</v>
+      </c>
+      <c r="E14" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="F14" s="3">
+        <v>100</v>
+      </c>
+      <c r="G14" s="3">
+        <v>732</v>
+      </c>
+      <c r="H14" s="3">
+        <v>7.32</v>
+      </c>
+    </row>
+    <row r="15" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C15" s="3">
+        <v>100</v>
+      </c>
+      <c r="D15" s="3">
         <v>3</v>
       </c>
-      <c r="E14" s="13">
+      <c r="E15" s="10">
         <v>0.03</v>
       </c>
-      <c r="F14" s="3">
-        <v>100</v>
-      </c>
-      <c r="G14" s="3">
+      <c r="F15" s="3">
+        <v>100</v>
+      </c>
+      <c r="G15" s="3">
         <v>675</v>
       </c>
-      <c r="H14" s="3">
+      <c r="H15" s="3">
         <v>6.75</v>
+      </c>
+    </row>
+    <row r="16" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C16" s="3">
+        <v>100</v>
+      </c>
+      <c r="D16" s="3">
+        <v>3</v>
+      </c>
+      <c r="E16" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F16" s="3">
+        <v>100</v>
+      </c>
+      <c r="G16" s="3">
+        <v>916</v>
+      </c>
+      <c r="H16" s="3">
+        <v>9.16</v>
+      </c>
+    </row>
+    <row r="17" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B17" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="C17" s="3">
+        <v>100</v>
+      </c>
+      <c r="D17" s="3">
+        <v>0</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0</v>
+      </c>
+      <c r="F17" s="3">
+        <v>100</v>
+      </c>
+      <c r="G17" s="3">
+        <v>1021</v>
+      </c>
+      <c r="H17" s="3">
+        <v>10.210000000000001</v>
       </c>
     </row>
   </sheetData>
@@ -2369,10 +2715,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15506EA-4930-9441-B4F3-EDD7A1FF6E26}">
-  <dimension ref="B2:F25"/>
+  <dimension ref="B2:F31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="136" workbookViewId="0">
-      <selection activeCell="G12" sqref="G12"/>
+    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
+      <selection activeCell="J18" sqref="J18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2384,394 +2730,493 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="16" t="s">
+      <c r="C2" s="36" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="16"/>
-      <c r="E2" s="16"/>
-      <c r="F2" s="16"/>
+      <c r="D2" s="36"/>
+      <c r="E2" s="36"/>
+      <c r="F2" s="36"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
       <c r="C3" s="3" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="17" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" s="11" t="s">
         <v>0</v>
       </c>
-      <c r="E3" s="17" t="s">
+      <c r="E3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="F3" s="17" t="s">
+      <c r="F3" s="11" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="41" t="s">
+      <c r="B4" s="37" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="42" t="s">
-        <v>17</v>
-      </c>
-      <c r="D4" s="43">
-        <v>150</v>
-      </c>
-      <c r="E4" s="43">
+      <c r="C4" s="27" t="s">
+        <v>16</v>
+      </c>
+      <c r="D4" s="28">
+        <v>150</v>
+      </c>
+      <c r="E4" s="28">
         <v>96</v>
       </c>
-      <c r="F4" s="44">
+      <c r="F4" s="29">
         <v>0.64</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="45"/>
-      <c r="C5" s="42" t="s">
+      <c r="B5" s="38"/>
+      <c r="C5" s="27" t="s">
+        <v>15</v>
+      </c>
+      <c r="D5" s="28">
+        <v>100</v>
+      </c>
+      <c r="E5" s="28">
+        <v>71</v>
+      </c>
+      <c r="F5" s="29">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B6" s="39" t="s">
+        <v>12</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>16</v>
       </c>
-      <c r="D5" s="43">
-        <v>100</v>
-      </c>
-      <c r="E5" s="43">
+      <c r="D6" s="13">
+        <v>150</v>
+      </c>
+      <c r="E6" s="13">
+        <v>107</v>
+      </c>
+      <c r="F6" s="14">
+        <v>0.71330000000000005</v>
+      </c>
+    </row>
+    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B7" s="40"/>
+      <c r="C7" s="12" t="s">
+        <v>15</v>
+      </c>
+      <c r="D7" s="13">
+        <v>100</v>
+      </c>
+      <c r="E7" s="13">
+        <v>74</v>
+      </c>
+      <c r="F7" s="14">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B8" s="41" t="s">
+        <v>13</v>
+      </c>
+      <c r="C8" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D8" s="16">
+        <v>150</v>
+      </c>
+      <c r="E8" s="16">
+        <v>85</v>
+      </c>
+      <c r="F8" s="17">
+        <v>0.56659999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B9" s="42"/>
+      <c r="C9" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D9" s="16">
+        <v>100</v>
+      </c>
+      <c r="E9" s="16">
         <v>71</v>
       </c>
-      <c r="F5" s="44">
+      <c r="F9" s="17">
         <v>0.71</v>
       </c>
     </row>
-    <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="18" t="s">
-        <v>12</v>
-      </c>
-      <c r="C6" s="19" t="s">
-        <v>17</v>
-      </c>
-      <c r="D6" s="20">
-        <v>150</v>
-      </c>
-      <c r="E6" s="20">
-        <v>107</v>
-      </c>
-      <c r="F6" s="21">
-        <v>0.71330000000000005</v>
-      </c>
-    </row>
-    <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="22"/>
-      <c r="C7" s="19" t="s">
+    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B10" s="43" t="s">
+        <v>14</v>
+      </c>
+      <c r="C10" s="21" t="s">
         <v>16</v>
       </c>
-      <c r="D7" s="20">
-        <v>100</v>
-      </c>
-      <c r="E7" s="20">
+      <c r="D10" s="22">
+        <v>150</v>
+      </c>
+      <c r="E10" s="22">
+        <v>102</v>
+      </c>
+      <c r="F10" s="23">
+        <v>0.68</v>
+      </c>
+    </row>
+    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B11" s="44"/>
+      <c r="C11" s="21" t="s">
+        <v>15</v>
+      </c>
+      <c r="D11" s="22">
+        <v>100</v>
+      </c>
+      <c r="E11" s="22">
+        <v>77</v>
+      </c>
+      <c r="F11" s="23">
+        <v>0.77</v>
+      </c>
+    </row>
+    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B12" s="34" t="s">
+        <v>29</v>
+      </c>
+      <c r="C12" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D12" s="25">
+        <v>150</v>
+      </c>
+      <c r="E12" s="25">
+        <v>90</v>
+      </c>
+      <c r="F12" s="26">
+        <v>0.6</v>
+      </c>
+    </row>
+    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B13" s="35"/>
+      <c r="C13" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D13" s="25">
+        <v>100</v>
+      </c>
+      <c r="E13" s="25">
+        <v>67</v>
+      </c>
+      <c r="F13" s="26">
+        <v>0.67</v>
+      </c>
+    </row>
+    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B14" s="34" t="s">
+        <v>20</v>
+      </c>
+      <c r="C14" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D14" s="25">
+        <v>150</v>
+      </c>
+      <c r="E14" s="25">
+        <v>100</v>
+      </c>
+      <c r="F14" s="26">
+        <v>0.66669999999999996</v>
+      </c>
+    </row>
+    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B15" s="35"/>
+      <c r="C15" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D15" s="25">
+        <v>100</v>
+      </c>
+      <c r="E15" s="25">
+        <v>76</v>
+      </c>
+      <c r="F15" s="26">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B16" s="34" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D16" s="25">
+        <v>150</v>
+      </c>
+      <c r="E16" s="25">
+        <v>97</v>
+      </c>
+      <c r="F16" s="26">
+        <v>0.64670000000000005</v>
+      </c>
+    </row>
+    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B17" s="35"/>
+      <c r="C17" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17" s="25">
+        <v>100</v>
+      </c>
+      <c r="E17" s="25">
         <v>74</v>
       </c>
-      <c r="F7" s="21">
+      <c r="F17" s="26">
         <v>0.74</v>
       </c>
     </row>
-    <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="23" t="s">
-        <v>13</v>
-      </c>
-      <c r="C8" s="24" t="s">
-        <v>17</v>
-      </c>
-      <c r="D8" s="25">
-        <v>150</v>
-      </c>
-      <c r="E8" s="25">
-        <v>85</v>
-      </c>
-      <c r="F8" s="26">
-        <v>0.56659999999999999</v>
-      </c>
-    </row>
-    <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="27"/>
-      <c r="C9" s="24" t="s">
+    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B18" s="34" t="s">
+        <v>22</v>
+      </c>
+      <c r="C18" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D9" s="25">
-        <v>100</v>
-      </c>
-      <c r="E9" s="25">
-        <v>71</v>
-      </c>
-      <c r="F9" s="26">
-        <v>0.71</v>
-      </c>
-    </row>
-    <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="31" t="s">
-        <v>14</v>
-      </c>
-      <c r="C10" s="32" t="s">
-        <v>17</v>
-      </c>
-      <c r="D10" s="33">
-        <v>150</v>
-      </c>
-      <c r="E10" s="33">
+      <c r="D18" s="25">
+        <v>150</v>
+      </c>
+      <c r="E18" s="25">
         <v>102</v>
       </c>
-      <c r="F10" s="34">
+      <c r="F18" s="26">
         <v>0.68</v>
       </c>
     </row>
-    <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="35"/>
-      <c r="C11" s="32" t="s">
+    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B19" s="35"/>
+      <c r="C19" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D19" s="25">
+        <v>100</v>
+      </c>
+      <c r="E19" s="25">
+        <v>74</v>
+      </c>
+      <c r="F19" s="26">
+        <v>0.74</v>
+      </c>
+    </row>
+    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B20" s="34" t="s">
+        <v>23</v>
+      </c>
+      <c r="C20" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="D11" s="33">
-        <v>100</v>
-      </c>
-      <c r="E11" s="33">
+      <c r="D20" s="25">
+        <v>150</v>
+      </c>
+      <c r="E20" s="25">
+        <v>98</v>
+      </c>
+      <c r="F20" s="26">
+        <v>0.65329999999999999</v>
+      </c>
+    </row>
+    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B21" s="35"/>
+      <c r="C21" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D21" s="25">
+        <v>100</v>
+      </c>
+      <c r="E21" s="25">
+        <v>69</v>
+      </c>
+      <c r="F21" s="26">
+        <v>0.69</v>
+      </c>
+    </row>
+    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B22" s="32" t="s">
+        <v>24</v>
+      </c>
+      <c r="C22" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D22" s="25">
+        <v>150</v>
+      </c>
+      <c r="E22" s="25">
+        <v>112</v>
+      </c>
+      <c r="F22" s="26">
+        <v>0.74670000000000003</v>
+      </c>
+    </row>
+    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B23" s="33"/>
+      <c r="C23" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D23" s="25">
+        <v>100</v>
+      </c>
+      <c r="E23" s="25">
+        <v>75</v>
+      </c>
+      <c r="F23" s="26">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B24" s="32" t="s">
+        <v>25</v>
+      </c>
+      <c r="C24" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D24" s="25">
+        <v>150</v>
+      </c>
+      <c r="E24" s="25">
+        <v>116</v>
+      </c>
+      <c r="F24" s="26">
+        <v>0.77329999999999999</v>
+      </c>
+    </row>
+    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B25" s="33"/>
+      <c r="C25" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D25" s="25">
+        <v>100</v>
+      </c>
+      <c r="E25" s="25">
+        <v>73</v>
+      </c>
+      <c r="F25" s="26">
+        <v>0.73</v>
+      </c>
+    </row>
+    <row r="26" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B26" s="32" t="s">
+        <v>26</v>
+      </c>
+      <c r="C26" s="24" t="s">
+        <v>16</v>
+      </c>
+      <c r="D26" s="25">
+        <v>150</v>
+      </c>
+      <c r="E26" s="25">
+        <v>118</v>
+      </c>
+      <c r="F26" s="26">
+        <v>0.78669999999999995</v>
+      </c>
+    </row>
+    <row r="27" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B27" s="33"/>
+      <c r="C27" s="24" t="s">
+        <v>15</v>
+      </c>
+      <c r="D27" s="25">
+        <v>100</v>
+      </c>
+      <c r="E27" s="25">
         <v>77</v>
       </c>
-      <c r="F11" s="34">
+      <c r="F27" s="26">
         <v>0.77</v>
       </c>
     </row>
-    <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="36" t="s">
+    <row r="28" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B28" s="50" t="s">
+        <v>27</v>
+      </c>
+      <c r="C28" s="51" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="52">
+        <v>150</v>
+      </c>
+      <c r="E28" s="52">
+        <v>119</v>
+      </c>
+      <c r="F28" s="53">
+        <v>0.79330000000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="54"/>
+      <c r="C29" s="51" t="s">
         <v>15</v>
       </c>
-      <c r="C12" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D12" s="38">
-        <v>150</v>
-      </c>
-      <c r="E12" s="38">
-        <v>100</v>
-      </c>
-      <c r="F12" s="39">
-        <v>0.66669999999999996</v>
-      </c>
-    </row>
-    <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="40"/>
-      <c r="C13" s="37" t="s">
+      <c r="D29" s="52">
+        <v>100</v>
+      </c>
+      <c r="E29" s="52">
+        <v>83</v>
+      </c>
+      <c r="F29" s="53">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="55" t="s">
+        <v>28</v>
+      </c>
+      <c r="C30" s="56" t="s">
         <v>16</v>
       </c>
-      <c r="D13" s="38">
-        <v>100</v>
-      </c>
-      <c r="E13" s="38">
-        <v>76</v>
-      </c>
-      <c r="F13" s="39">
-        <v>0.76</v>
-      </c>
-    </row>
-    <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="36" t="s">
-        <v>19</v>
-      </c>
-      <c r="C14" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D14" s="38">
-        <v>150</v>
-      </c>
-      <c r="E14" s="38">
-        <v>97</v>
-      </c>
-      <c r="F14" s="39">
-        <v>0.64670000000000005</v>
-      </c>
-    </row>
-    <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="40"/>
-      <c r="C15" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D15" s="38">
-        <v>100</v>
-      </c>
-      <c r="E15" s="38">
-        <v>74</v>
-      </c>
-      <c r="F15" s="39">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="36" t="s">
-        <v>20</v>
-      </c>
-      <c r="C16" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D16" s="38">
-        <v>150</v>
-      </c>
-      <c r="E16" s="38">
-        <v>102</v>
-      </c>
-      <c r="F16" s="39">
-        <v>0.68</v>
-      </c>
-    </row>
-    <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="40"/>
-      <c r="C17" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D17" s="38">
-        <v>100</v>
-      </c>
-      <c r="E17" s="38">
-        <v>74</v>
-      </c>
-      <c r="F17" s="39">
-        <v>0.74</v>
-      </c>
-    </row>
-    <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="36" t="s">
-        <v>21</v>
-      </c>
-      <c r="C18" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D18" s="38">
-        <v>150</v>
-      </c>
-      <c r="E18" s="38">
-        <v>98</v>
-      </c>
-      <c r="F18" s="39">
-        <v>0.65329999999999999</v>
-      </c>
-    </row>
-    <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="40"/>
-      <c r="C19" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D19" s="38">
-        <v>100</v>
-      </c>
-      <c r="E19" s="38">
-        <v>69</v>
-      </c>
-      <c r="F19" s="39">
-        <v>0.69</v>
-      </c>
-    </row>
-    <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="47" t="s">
-        <v>22</v>
-      </c>
-      <c r="C20" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D20" s="38">
-        <v>150</v>
-      </c>
-      <c r="E20" s="38">
+      <c r="D30" s="57">
+        <v>150</v>
+      </c>
+      <c r="E30" s="57">
         <v>112</v>
       </c>
-      <c r="F20" s="39">
+      <c r="F30" s="58">
         <v>0.74670000000000003</v>
       </c>
     </row>
-    <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="48"/>
-      <c r="C21" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D21" s="38">
-        <v>100</v>
-      </c>
-      <c r="E21" s="38">
-        <v>75</v>
-      </c>
-      <c r="F21" s="39">
-        <v>0.75</v>
-      </c>
-    </row>
-    <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="47" t="s">
-        <v>23</v>
-      </c>
-      <c r="C22" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D22" s="38">
-        <v>150</v>
-      </c>
-      <c r="E22" s="38">
-        <v>116</v>
-      </c>
-      <c r="F22" s="39">
-        <v>0.77329999999999999</v>
-      </c>
-    </row>
-    <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="48"/>
-      <c r="C23" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D23" s="38">
-        <v>100</v>
-      </c>
-      <c r="E23" s="38">
-        <v>73</v>
-      </c>
-      <c r="F23" s="39">
-        <v>0.73</v>
-      </c>
-    </row>
-    <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="47" t="s">
-        <v>24</v>
-      </c>
-      <c r="C24" s="37" t="s">
-        <v>17</v>
-      </c>
-      <c r="D24" s="38">
-        <v>150</v>
-      </c>
-      <c r="E24" s="38">
-        <v>118</v>
-      </c>
-      <c r="F24" s="39">
-        <v>0.78669999999999995</v>
-      </c>
-    </row>
-    <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="48"/>
-      <c r="C25" s="37" t="s">
-        <v>16</v>
-      </c>
-      <c r="D25" s="38">
-        <v>100</v>
-      </c>
-      <c r="E25" s="38">
-        <v>77</v>
-      </c>
-      <c r="F25" s="39">
-        <v>0.77</v>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="59"/>
+      <c r="C31" s="56" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="57">
+        <v>100</v>
+      </c>
+      <c r="E31" s="57">
+        <v>86</v>
+      </c>
+      <c r="F31" s="58">
+        <v>0.86</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="12">
-    <mergeCell ref="B24:B25"/>
+  <mergeCells count="15">
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
     <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B26:B27"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
     <mergeCell ref="B18:B19"/>
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
+    <mergeCell ref="B24:B25"/>
   </mergeCells>
   <phoneticPr fontId="3" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -2795,11 +3240,11 @@
     <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
-      <c r="C2" s="10" t="s">
+      <c r="C2" s="45" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="11"/>
-      <c r="E2" s="12"/>
+      <c r="D2" s="46"/>
+      <c r="E2" s="47"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="2"/>
@@ -2865,16 +3310,16 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="15" t="s">
+      <c r="C2" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="15"/>
-      <c r="E2" s="15"/>
-      <c r="F2" s="15" t="s">
+      <c r="D2" s="31"/>
+      <c r="E2" s="31"/>
+      <c r="F2" s="31" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="15"/>
-      <c r="H2" s="15"/>
+      <c r="G2" s="31"/>
+      <c r="H2" s="31"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -2907,7 +3352,7 @@
       <c r="D4" s="3">
         <v>7</v>
       </c>
-      <c r="E4" s="13">
+      <c r="E4" s="10">
         <v>2.8000000000000001E-2</v>
       </c>
       <c r="F4" s="3">
@@ -2930,7 +3375,7 @@
       <c r="D5" s="3">
         <v>0</v>
       </c>
-      <c r="E5" s="13">
+      <c r="E5" s="10">
         <v>0</v>
       </c>
       <c r="F5" s="3">

</xml_diff>

<commit_message>
codellamav8 sqlcoderv1 deepseekv1 eval
</commit_message>
<xml_diff>
--- a/evaluation/results_by_data_split.xlsx
+++ b/evaluation/results_by_data_split.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yufeizhao/Desktop/11667MiniProject/11667-NLP2SQL/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F569FA4-FB7C-F14E-9508-7A16899B31A0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{69DE8E71-EC2B-3548-A5BF-0D3EB0D85063}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-1700" yWindow="-20560" windowWidth="28040" windowHeight="19460" activeTab="5" xr2:uid="{44081516-0D10-9B41-9157-44A5B55A14F9}"/>
+    <workbookView xWindow="-360" yWindow="-21820" windowWidth="28040" windowHeight="19460" activeTab="2" xr2:uid="{44081516-0D10-9B41-9157-44A5B55A14F9}"/>
   </bookViews>
   <sheets>
     <sheet name="train_sql2sql" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="30">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="37">
   <si>
     <t>total queries</t>
   </si>
@@ -134,12 +134,33 @@
   <si>
     <t>promptv4_codellama_v0</t>
   </si>
+  <si>
+    <t>promptv4_codellama_v8</t>
+  </si>
+  <si>
+    <t>promptv4_codellama_v8.1</t>
+  </si>
+  <si>
+    <t>promptv4_codellama_v8.2</t>
+  </si>
+  <si>
+    <t>promptv3_deepseek_v1</t>
+  </si>
+  <si>
+    <t>promptv3_sqlcoder_v1</t>
+  </si>
+  <si>
+    <t>promptv4_deepseek_v1</t>
+  </si>
+  <si>
+    <t>promptv4_sqlcoder_v1</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -155,20 +176,13 @@
       <scheme val="minor"/>
     </font>
     <font>
-      <sz val="12"/>
-      <color rgb="FFFF0000"/>
-      <name val="Aptos Narrow"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
       <sz val="8"/>
       <name val="Aptos Narrow"/>
       <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="6">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -177,31 +191,7 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor theme="9" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="5" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="8" tint="0.79998168889431442"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="3" tint="0.89999084444715716"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor theme="2" tint="-9.9978637043366805E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -214,6 +204,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF8F5C3"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -408,7 +404,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="60">
+  <cellXfs count="45">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -443,6 +439,15 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -452,6 +457,12 @@
     <xf numFmtId="10" fontId="1" fillId="2" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -461,15 +472,6 @@
     <xf numFmtId="10" fontId="1" fillId="3" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="4" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -479,6 +481,48 @@
     <xf numFmtId="10" fontId="1" fillId="4" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -488,103 +532,10 @@
     <xf numFmtId="10" fontId="1" fillId="5" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="6" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="6" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="5" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="5" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="6" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="14" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="7" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="7" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="7" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="3" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="8" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="10" fontId="1" fillId="8" borderId="3" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="8" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -941,16 +892,16 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -1099,10 +1050,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C775F-3A5B-8346-B68B-D75012605A96}">
-  <dimension ref="B2:H19"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="C19" sqref="C19"/>
+      <selection activeCell="E25" sqref="E25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1113,16 +1064,16 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -1394,7 +1345,7 @@
       <c r="G14" s="3">
         <v>850</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="12">
         <v>3.4</v>
       </c>
     </row>
@@ -1469,48 +1420,163 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>18</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3">
         <v>250</v>
       </c>
       <c r="D18" s="3">
-        <v>55</v>
+        <v>127</v>
       </c>
       <c r="E18" s="10">
-        <v>0.22</v>
+        <v>0.50800000000000001</v>
       </c>
       <c r="F18" s="3">
         <v>250</v>
       </c>
       <c r="G18" s="3">
-        <v>1657</v>
+        <v>809</v>
       </c>
       <c r="H18" s="3">
-        <v>6.63</v>
+        <v>3.24</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3">
+        <v>250</v>
+      </c>
+      <c r="D19" s="3">
+        <v>123</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="F19" s="3">
+        <v>250</v>
+      </c>
+      <c r="G19" s="3">
+        <v>827</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3.31</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="3">
+        <v>250</v>
+      </c>
+      <c r="D20" s="3">
+        <v>118</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.47199999999999998</v>
+      </c>
+      <c r="F20" s="3">
+        <v>250</v>
+      </c>
+      <c r="G20" s="3">
+        <v>847</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3.39</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="C21" s="3">
+        <v>250</v>
+      </c>
+      <c r="D21" s="3">
+        <v>55</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.22</v>
+      </c>
+      <c r="F21" s="3">
+        <v>250</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1657</v>
+      </c>
+      <c r="H21" s="3">
+        <v>6.63</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="C22" s="3">
+        <v>250</v>
+      </c>
+      <c r="D22" s="3">
+        <v>122</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0.48799999999999999</v>
+      </c>
+      <c r="F22" s="3">
+        <v>250</v>
+      </c>
+      <c r="G22" s="3">
+        <v>923</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3.69</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>19</v>
       </c>
-      <c r="C19" s="3">
-        <v>250</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="C23" s="3">
+        <v>250</v>
+      </c>
+      <c r="D23" s="3">
         <v>3</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E23" s="10">
         <v>1.2E-2</v>
       </c>
-      <c r="F19" s="3">
-        <v>250</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F23" s="3">
+        <v>250</v>
+      </c>
+      <c r="G23" s="3">
         <v>2292</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H23" s="3">
         <v>9.17</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="3">
+        <v>250</v>
+      </c>
+      <c r="D24" s="3">
+        <v>115</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.46</v>
+      </c>
+      <c r="F24" s="3">
+        <v>250</v>
+      </c>
+      <c r="G24" s="3">
+        <v>904</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3.62</v>
       </c>
     </row>
   </sheetData>
@@ -1518,17 +1584,17 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82A48FE-26B2-E846-83D1-3D5B61BC4083}">
-  <dimension ref="B2:H20"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
-    <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I9" sqref="I9"/>
+    <sheetView tabSelected="1" zoomScale="150" workbookViewId="0">
+      <selection activeCell="D10" sqref="D10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1539,16 +1605,16 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -1705,7 +1771,7 @@
       <c r="G9" s="3">
         <v>925</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="12">
         <v>3.7</v>
       </c>
     </row>
@@ -1725,10 +1791,10 @@
       <c r="F10" s="3">
         <v>250</v>
       </c>
-      <c r="G10" s="19">
+      <c r="G10" s="13">
         <v>1903</v>
       </c>
-      <c r="H10" s="48">
+      <c r="H10" s="18">
         <v>7.61</v>
       </c>
     </row>
@@ -1748,10 +1814,10 @@
       <c r="F11" s="3">
         <v>250</v>
       </c>
-      <c r="G11" s="19">
+      <c r="G11" s="13">
         <v>890</v>
       </c>
-      <c r="H11" s="19">
+      <c r="H11" s="13">
         <v>3.56</v>
       </c>
     </row>
@@ -1774,7 +1840,7 @@
       <c r="G12" s="3">
         <v>899</v>
       </c>
-      <c r="H12" s="18">
+      <c r="H12" s="12">
         <v>3.6</v>
       </c>
     </row>
@@ -1820,7 +1886,7 @@
       <c r="G14" s="3">
         <v>876</v>
       </c>
-      <c r="H14" s="18">
+      <c r="H14" s="12">
         <v>3.5</v>
       </c>
     </row>
@@ -1854,10 +1920,10 @@
       <c r="C16" s="3">
         <v>250</v>
       </c>
-      <c r="D16" s="19">
+      <c r="D16" s="13">
         <v>125</v>
       </c>
-      <c r="E16" s="20">
+      <c r="E16" s="14">
         <v>0.5</v>
       </c>
       <c r="F16" s="3">
@@ -1895,90 +1961,201 @@
     </row>
     <row r="18" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B18" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C18" s="3">
         <v>250</v>
       </c>
       <c r="D18" s="3">
-        <v>58</v>
+        <v>142</v>
       </c>
       <c r="E18" s="10">
-        <v>0.23200000000000001</v>
+        <v>0.56799999999999995</v>
       </c>
       <c r="F18" s="3">
         <v>250</v>
       </c>
       <c r="G18" s="3">
-        <v>1677</v>
+        <v>793</v>
       </c>
       <c r="H18" s="3">
-        <v>6.71</v>
+        <v>3.17</v>
       </c>
     </row>
     <row r="19" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B19" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C19" s="3">
+        <v>250</v>
+      </c>
+      <c r="D19" s="3">
+        <v>141</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.56399999999999995</v>
+      </c>
+      <c r="F19" s="3">
+        <v>250</v>
+      </c>
+      <c r="G19" s="3">
+        <v>812</v>
+      </c>
+      <c r="H19" s="3">
+        <v>3.25</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C20" s="3">
+        <v>250</v>
+      </c>
+      <c r="D20" s="3">
+        <v>128</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.51200000000000001</v>
+      </c>
+      <c r="F20" s="3">
+        <v>250</v>
+      </c>
+      <c r="G20" s="3">
+        <v>918</v>
+      </c>
+      <c r="H20" s="3">
+        <v>3.67</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C21" s="3">
+        <v>250</v>
+      </c>
+      <c r="D21" s="3">
+        <v>58</v>
+      </c>
+      <c r="E21" s="10">
+        <v>0.23200000000000001</v>
+      </c>
+      <c r="F21" s="3">
+        <v>250</v>
+      </c>
+      <c r="G21" s="3">
+        <v>1677</v>
+      </c>
+      <c r="H21" s="3">
+        <v>6.71</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C22" s="3">
+        <v>250</v>
+      </c>
+      <c r="D22" s="3">
+        <v>129</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0.51600000000000001</v>
+      </c>
+      <c r="F22" s="3">
+        <v>250</v>
+      </c>
+      <c r="G22" s="3">
+        <v>940</v>
+      </c>
+      <c r="H22" s="3">
+        <v>3.76</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C19" s="3">
-        <v>250</v>
-      </c>
-      <c r="D19" s="3">
+      <c r="C23" s="3">
+        <v>250</v>
+      </c>
+      <c r="D23" s="3">
         <v>2</v>
       </c>
-      <c r="E19" s="10">
+      <c r="E23" s="10">
         <v>8.0000000000000002E-3</v>
       </c>
-      <c r="F19" s="3">
-        <v>250</v>
-      </c>
-      <c r="G19" s="3">
+      <c r="F23" s="3">
+        <v>250</v>
+      </c>
+      <c r="G23" s="3">
         <v>2273</v>
       </c>
-      <c r="H19" s="3">
+      <c r="H23" s="3">
         <v>9.09</v>
       </c>
     </row>
-    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="D20" s="49"/>
-      <c r="E20" s="49"/>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C24" s="3">
+        <v>250</v>
+      </c>
+      <c r="D24" s="3">
+        <v>123</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="F24" s="3">
+        <v>250</v>
+      </c>
+      <c r="G24" s="3">
+        <v>910</v>
+      </c>
+      <c r="H24" s="3">
+        <v>3.64</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA613D23-B9DE-0542-95AA-364F896410C8}">
-  <dimension ref="B2:H17"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="I18" sqref="I18"/>
+      <selection activeCell="B14" sqref="B14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="8" width="12.83203125" style="49" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -2135,7 +2312,7 @@
       <c r="G9" s="3">
         <v>660</v>
       </c>
-      <c r="H9" s="18">
+      <c r="H9" s="12">
         <v>4.4000000000000004</v>
       </c>
     </row>
@@ -2209,7 +2386,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="44" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="3">
@@ -2279,48 +2456,163 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3">
         <v>150</v>
       </c>
       <c r="D16" s="3">
-        <v>3</v>
+        <v>24</v>
       </c>
       <c r="E16" s="10">
-        <v>0.02</v>
+        <v>0.16</v>
       </c>
       <c r="F16" s="3">
         <v>150</v>
       </c>
       <c r="G16" s="3">
-        <v>1605</v>
+        <v>422</v>
       </c>
       <c r="H16" s="3">
-        <v>10.7</v>
+        <v>2.81</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3">
+        <v>150</v>
+      </c>
+      <c r="D17" s="3">
+        <v>24</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.16</v>
+      </c>
+      <c r="F17" s="3">
+        <v>150</v>
+      </c>
+      <c r="G17" s="3">
+        <v>417</v>
+      </c>
+      <c r="H17" s="3">
+        <v>2.78</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3">
+        <v>150</v>
+      </c>
+      <c r="D18" s="3">
+        <v>19</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.12670000000000001</v>
+      </c>
+      <c r="F18" s="3">
+        <v>150</v>
+      </c>
+      <c r="G18" s="3">
+        <v>641</v>
+      </c>
+      <c r="H18" s="3">
+        <v>4.2699999999999996</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3">
+        <v>150</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.02</v>
+      </c>
+      <c r="F19" s="3">
+        <v>150</v>
+      </c>
+      <c r="G19" s="3">
+        <v>1605</v>
+      </c>
+      <c r="H19" s="3">
+        <v>10.7</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3">
+        <v>150</v>
+      </c>
+      <c r="D20" s="3">
+        <v>14</v>
+      </c>
+      <c r="E20" s="10">
+        <v>9.3299999999999994E-2</v>
+      </c>
+      <c r="F20" s="3">
+        <v>150</v>
+      </c>
+      <c r="G20" s="3">
+        <v>774</v>
+      </c>
+      <c r="H20" s="3">
+        <v>5.16</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3">
-        <v>150</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="C21" s="3">
+        <v>150</v>
+      </c>
+      <c r="D21" s="3">
         <v>0</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E21" s="10">
         <v>0</v>
       </c>
-      <c r="F17" s="3">
-        <v>150</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="F21" s="3">
+        <v>150</v>
+      </c>
+      <c r="G21" s="3">
         <v>1728</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H21" s="3">
         <v>11.52</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3">
+        <v>150</v>
+      </c>
+      <c r="D22" s="3">
+        <v>10</v>
+      </c>
+      <c r="E22" s="10">
+        <v>6.6699999999999995E-2</v>
+      </c>
+      <c r="F22" s="3">
+        <v>150</v>
+      </c>
+      <c r="G22" s="3">
+        <v>772</v>
+      </c>
+      <c r="H22" s="3">
+        <v>5.15</v>
       </c>
     </row>
   </sheetData>
@@ -2328,37 +2620,37 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C74F51-BDAD-924D-AEFA-68C8E4D340A8}">
-  <dimension ref="B2:H17"/>
+  <dimension ref="B2:H22"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="E24" sqref="E24"/>
+      <selection activeCell="C22" sqref="C22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="22.83203125" customWidth="1"/>
-    <col min="3" max="8" width="12.83203125" style="49" customWidth="1"/>
+    <col min="3" max="8" width="12.83203125" style="19" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -2589,7 +2881,7 @@
       </c>
     </row>
     <row r="13" spans="2:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="30" t="s">
+      <c r="B13" s="44" t="s">
         <v>24</v>
       </c>
       <c r="C13" s="3">
@@ -2659,48 +2951,163 @@
     </row>
     <row r="16" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B16" s="3" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="C16" s="3">
         <v>100</v>
       </c>
       <c r="D16" s="3">
-        <v>3</v>
+        <v>4</v>
       </c>
       <c r="E16" s="10">
-        <v>0.03</v>
+        <v>0.04</v>
       </c>
       <c r="F16" s="3">
         <v>100</v>
       </c>
       <c r="G16" s="3">
-        <v>916</v>
+        <v>673</v>
       </c>
       <c r="H16" s="3">
-        <v>9.16</v>
+        <v>6.73</v>
       </c>
     </row>
     <row r="17" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B17" s="3" t="s">
+        <v>31</v>
+      </c>
+      <c r="C17" s="3">
+        <v>100</v>
+      </c>
+      <c r="D17" s="3">
+        <v>4</v>
+      </c>
+      <c r="E17" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F17" s="3">
+        <v>100</v>
+      </c>
+      <c r="G17" s="3">
+        <v>699</v>
+      </c>
+      <c r="H17" s="3">
+        <v>6.99</v>
+      </c>
+    </row>
+    <row r="18" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B18" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="C18" s="3">
+        <v>100</v>
+      </c>
+      <c r="D18" s="3">
+        <v>3</v>
+      </c>
+      <c r="E18" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F18" s="3">
+        <v>100</v>
+      </c>
+      <c r="G18" s="3">
+        <v>709</v>
+      </c>
+      <c r="H18" s="3">
+        <v>7.09</v>
+      </c>
+    </row>
+    <row r="19" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B19" s="3" t="s">
+        <v>27</v>
+      </c>
+      <c r="C19" s="3">
+        <v>100</v>
+      </c>
+      <c r="D19" s="3">
+        <v>3</v>
+      </c>
+      <c r="E19" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F19" s="3">
+        <v>100</v>
+      </c>
+      <c r="G19" s="3">
+        <v>916</v>
+      </c>
+      <c r="H19" s="3">
+        <v>9.16</v>
+      </c>
+    </row>
+    <row r="20" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B20" s="3" t="s">
+        <v>35</v>
+      </c>
+      <c r="C20" s="3">
+        <v>100</v>
+      </c>
+      <c r="D20" s="3">
+        <v>6</v>
+      </c>
+      <c r="E20" s="10">
+        <v>0.06</v>
+      </c>
+      <c r="F20" s="3">
+        <v>100</v>
+      </c>
+      <c r="G20" s="3">
+        <v>698</v>
+      </c>
+      <c r="H20" s="3">
+        <v>6.98</v>
+      </c>
+    </row>
+    <row r="21" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B21" s="3" t="s">
         <v>28</v>
       </c>
-      <c r="C17" s="3">
-        <v>100</v>
-      </c>
-      <c r="D17" s="3">
+      <c r="C21" s="3">
+        <v>100</v>
+      </c>
+      <c r="D21" s="3">
         <v>0</v>
       </c>
-      <c r="E17" s="10">
+      <c r="E21" s="10">
         <v>0</v>
       </c>
-      <c r="F17" s="3">
-        <v>100</v>
-      </c>
-      <c r="G17" s="3">
+      <c r="F21" s="3">
+        <v>100</v>
+      </c>
+      <c r="G21" s="3">
         <v>1021</v>
       </c>
-      <c r="H17" s="3">
+      <c r="H21" s="3">
         <v>10.210000000000001</v>
+      </c>
+    </row>
+    <row r="22" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B22" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="C22" s="3">
+        <v>100</v>
+      </c>
+      <c r="D22" s="3">
+        <v>4</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0.04</v>
+      </c>
+      <c r="F22" s="3">
+        <v>100</v>
+      </c>
+      <c r="G22" s="3">
+        <v>655</v>
+      </c>
+      <c r="H22" s="3">
+        <v>6.55</v>
       </c>
     </row>
   </sheetData>
@@ -2708,17 +3115,17 @@
     <mergeCell ref="C2:E2"/>
     <mergeCell ref="F2:H2"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15506EA-4930-9441-B4F3-EDD7A1FF6E26}">
-  <dimension ref="B2:F31"/>
+  <dimension ref="B2:F41"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="125" workbookViewId="0">
-      <selection activeCell="J18" sqref="J18"/>
+    <sheetView topLeftCell="A13" zoomScale="125" workbookViewId="0">
+      <selection activeCell="F27" sqref="F27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2730,12 +3137,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="33" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="33"/>
+      <c r="E2" s="33"/>
+      <c r="F2" s="33"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -2753,34 +3160,34 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="39" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="27" t="s">
+      <c r="C4" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D4" s="28">
-        <v>150</v>
-      </c>
-      <c r="E4" s="28">
+      <c r="D4" s="41">
+        <v>150</v>
+      </c>
+      <c r="E4" s="41">
         <v>96</v>
       </c>
-      <c r="F4" s="29">
+      <c r="F4" s="42">
         <v>0.64</v>
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="38"/>
-      <c r="C5" s="27" t="s">
+      <c r="B5" s="43"/>
+      <c r="C5" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D5" s="28">
-        <v>100</v>
-      </c>
-      <c r="E5" s="28">
+      <c r="D5" s="41">
+        <v>100</v>
+      </c>
+      <c r="E5" s="41">
         <v>71</v>
       </c>
-      <c r="F5" s="29">
+      <c r="F5" s="42">
         <v>0.71</v>
       </c>
     </row>
@@ -2788,422 +3195,586 @@
       <c r="B6" s="39" t="s">
         <v>12</v>
       </c>
-      <c r="C6" s="12" t="s">
+      <c r="C6" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D6" s="13">
-        <v>150</v>
-      </c>
-      <c r="E6" s="13">
+      <c r="D6" s="41">
+        <v>150</v>
+      </c>
+      <c r="E6" s="41">
         <v>107</v>
       </c>
-      <c r="F6" s="14">
+      <c r="F6" s="42">
         <v>0.71330000000000005</v>
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="40"/>
-      <c r="C7" s="12" t="s">
+      <c r="B7" s="43"/>
+      <c r="C7" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D7" s="13">
-        <v>100</v>
-      </c>
-      <c r="E7" s="13">
+      <c r="D7" s="41">
+        <v>100</v>
+      </c>
+      <c r="E7" s="41">
         <v>74</v>
       </c>
-      <c r="F7" s="14">
+      <c r="F7" s="42">
         <v>0.74</v>
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="41" t="s">
+      <c r="B8" s="39" t="s">
         <v>13</v>
       </c>
-      <c r="C8" s="15" t="s">
+      <c r="C8" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D8" s="16">
-        <v>150</v>
-      </c>
-      <c r="E8" s="16">
+      <c r="D8" s="41">
+        <v>150</v>
+      </c>
+      <c r="E8" s="41">
         <v>85</v>
       </c>
-      <c r="F8" s="17">
+      <c r="F8" s="42">
         <v>0.56659999999999999</v>
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="42"/>
-      <c r="C9" s="15" t="s">
+      <c r="B9" s="43"/>
+      <c r="C9" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D9" s="16">
-        <v>100</v>
-      </c>
-      <c r="E9" s="16">
+      <c r="D9" s="41">
+        <v>100</v>
+      </c>
+      <c r="E9" s="41">
         <v>71</v>
       </c>
-      <c r="F9" s="17">
+      <c r="F9" s="42">
         <v>0.71</v>
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="43" t="s">
+      <c r="B10" s="39" t="s">
         <v>14</v>
       </c>
-      <c r="C10" s="21" t="s">
+      <c r="C10" s="40" t="s">
         <v>16</v>
       </c>
-      <c r="D10" s="22">
-        <v>150</v>
-      </c>
-      <c r="E10" s="22">
+      <c r="D10" s="41">
+        <v>150</v>
+      </c>
+      <c r="E10" s="41">
         <v>102</v>
       </c>
-      <c r="F10" s="23">
+      <c r="F10" s="42">
         <v>0.68</v>
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="44"/>
-      <c r="C11" s="21" t="s">
+      <c r="B11" s="43"/>
+      <c r="C11" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="D11" s="22">
-        <v>100</v>
-      </c>
-      <c r="E11" s="22">
+      <c r="D11" s="41">
+        <v>100</v>
+      </c>
+      <c r="E11" s="41">
         <v>77</v>
       </c>
-      <c r="F11" s="23">
+      <c r="F11" s="42">
         <v>0.77</v>
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="34" t="s">
+      <c r="B12" s="31" t="s">
         <v>29</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D12" s="25">
-        <v>150</v>
-      </c>
-      <c r="E12" s="25">
+      <c r="D12" s="16">
+        <v>150</v>
+      </c>
+      <c r="E12" s="16">
         <v>90</v>
       </c>
-      <c r="F12" s="26">
+      <c r="F12" s="17">
         <v>0.6</v>
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="35"/>
-      <c r="C13" s="24" t="s">
+      <c r="B13" s="32"/>
+      <c r="C13" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D13" s="25">
-        <v>100</v>
-      </c>
-      <c r="E13" s="25">
+      <c r="D13" s="16">
+        <v>100</v>
+      </c>
+      <c r="E13" s="16">
         <v>67</v>
       </c>
-      <c r="F13" s="26">
+      <c r="F13" s="17">
         <v>0.67</v>
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="34" t="s">
+      <c r="B14" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="C14" s="24" t="s">
+      <c r="C14" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D14" s="25">
-        <v>150</v>
-      </c>
-      <c r="E14" s="25">
-        <v>100</v>
-      </c>
-      <c r="F14" s="26">
+      <c r="D14" s="16">
+        <v>150</v>
+      </c>
+      <c r="E14" s="16">
+        <v>100</v>
+      </c>
+      <c r="F14" s="17">
         <v>0.66669999999999996</v>
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="35"/>
-      <c r="C15" s="24" t="s">
+      <c r="B15" s="32"/>
+      <c r="C15" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D15" s="25">
-        <v>100</v>
-      </c>
-      <c r="E15" s="25">
+      <c r="D15" s="16">
+        <v>100</v>
+      </c>
+      <c r="E15" s="16">
         <v>76</v>
       </c>
-      <c r="F15" s="26">
+      <c r="F15" s="17">
         <v>0.76</v>
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="34" t="s">
+      <c r="B16" s="31" t="s">
         <v>21</v>
       </c>
-      <c r="C16" s="24" t="s">
+      <c r="C16" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D16" s="25">
-        <v>150</v>
-      </c>
-      <c r="E16" s="25">
+      <c r="D16" s="16">
+        <v>150</v>
+      </c>
+      <c r="E16" s="16">
         <v>97</v>
       </c>
-      <c r="F16" s="26">
+      <c r="F16" s="17">
         <v>0.64670000000000005</v>
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="35"/>
-      <c r="C17" s="24" t="s">
+      <c r="B17" s="32"/>
+      <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D17" s="25">
-        <v>100</v>
-      </c>
-      <c r="E17" s="25">
+      <c r="D17" s="16">
+        <v>100</v>
+      </c>
+      <c r="E17" s="16">
         <v>74</v>
       </c>
-      <c r="F17" s="26">
+      <c r="F17" s="17">
         <v>0.74</v>
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="34" t="s">
+      <c r="B18" s="31" t="s">
         <v>22</v>
       </c>
-      <c r="C18" s="24" t="s">
+      <c r="C18" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D18" s="25">
-        <v>150</v>
-      </c>
-      <c r="E18" s="25">
+      <c r="D18" s="16">
+        <v>150</v>
+      </c>
+      <c r="E18" s="16">
         <v>102</v>
       </c>
-      <c r="F18" s="26">
+      <c r="F18" s="17">
         <v>0.68</v>
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="35"/>
-      <c r="C19" s="24" t="s">
+      <c r="B19" s="32"/>
+      <c r="C19" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D19" s="25">
-        <v>100</v>
-      </c>
-      <c r="E19" s="25">
+      <c r="D19" s="16">
+        <v>100</v>
+      </c>
+      <c r="E19" s="16">
         <v>74</v>
       </c>
-      <c r="F19" s="26">
+      <c r="F19" s="17">
         <v>0.74</v>
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="34" t="s">
+      <c r="B20" s="31" t="s">
         <v>23</v>
       </c>
-      <c r="C20" s="24" t="s">
+      <c r="C20" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D20" s="25">
-        <v>150</v>
-      </c>
-      <c r="E20" s="25">
+      <c r="D20" s="16">
+        <v>150</v>
+      </c>
+      <c r="E20" s="16">
         <v>98</v>
       </c>
-      <c r="F20" s="26">
+      <c r="F20" s="17">
         <v>0.65329999999999999</v>
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="35"/>
-      <c r="C21" s="24" t="s">
+      <c r="B21" s="32"/>
+      <c r="C21" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D21" s="25">
-        <v>100</v>
-      </c>
-      <c r="E21" s="25">
+      <c r="D21" s="16">
+        <v>100</v>
+      </c>
+      <c r="E21" s="16">
         <v>69</v>
       </c>
-      <c r="F21" s="26">
+      <c r="F21" s="17">
         <v>0.69</v>
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="37" t="s">
         <v>24</v>
       </c>
-      <c r="C22" s="24" t="s">
+      <c r="C22" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D22" s="25">
-        <v>150</v>
-      </c>
-      <c r="E22" s="25">
+      <c r="D22" s="16">
+        <v>150</v>
+      </c>
+      <c r="E22" s="16">
         <v>112</v>
       </c>
-      <c r="F22" s="26">
+      <c r="F22" s="17">
         <v>0.74670000000000003</v>
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="33"/>
-      <c r="C23" s="24" t="s">
+      <c r="B23" s="38"/>
+      <c r="C23" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D23" s="25">
-        <v>100</v>
-      </c>
-      <c r="E23" s="25">
+      <c r="D23" s="16">
+        <v>100</v>
+      </c>
+      <c r="E23" s="16">
         <v>75</v>
       </c>
-      <c r="F23" s="26">
+      <c r="F23" s="17">
         <v>0.75</v>
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="37" t="s">
         <v>25</v>
       </c>
-      <c r="C24" s="24" t="s">
+      <c r="C24" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D24" s="25">
-        <v>150</v>
-      </c>
-      <c r="E24" s="25">
+      <c r="D24" s="16">
+        <v>150</v>
+      </c>
+      <c r="E24" s="16">
         <v>116</v>
       </c>
-      <c r="F24" s="26">
+      <c r="F24" s="17">
         <v>0.77329999999999999</v>
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="33"/>
-      <c r="C25" s="24" t="s">
+      <c r="B25" s="38"/>
+      <c r="C25" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D25" s="25">
-        <v>100</v>
-      </c>
-      <c r="E25" s="25">
+      <c r="D25" s="16">
+        <v>100</v>
+      </c>
+      <c r="E25" s="16">
         <v>73</v>
       </c>
-      <c r="F25" s="26">
+      <c r="F25" s="17">
         <v>0.73</v>
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="37" t="s">
         <v>26</v>
       </c>
-      <c r="C26" s="24" t="s">
+      <c r="C26" s="15" t="s">
         <v>16</v>
       </c>
-      <c r="D26" s="25">
-        <v>150</v>
-      </c>
-      <c r="E26" s="25">
+      <c r="D26" s="16">
+        <v>150</v>
+      </c>
+      <c r="E26" s="16">
         <v>118</v>
       </c>
-      <c r="F26" s="26">
+      <c r="F26" s="17">
         <v>0.78669999999999995</v>
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="33"/>
-      <c r="C27" s="24" t="s">
+      <c r="B27" s="38"/>
+      <c r="C27" s="15" t="s">
         <v>15</v>
       </c>
-      <c r="D27" s="25">
-        <v>100</v>
-      </c>
-      <c r="E27" s="25">
+      <c r="D27" s="16">
+        <v>100</v>
+      </c>
+      <c r="E27" s="16">
         <v>77</v>
       </c>
-      <c r="F27" s="26">
+      <c r="F27" s="17">
         <v>0.77</v>
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="50" t="s">
+      <c r="B28" s="37" t="s">
+        <v>30</v>
+      </c>
+      <c r="C28" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D28" s="16">
+        <v>150</v>
+      </c>
+      <c r="E28" s="16">
+        <v>137</v>
+      </c>
+      <c r="F28" s="17">
+        <v>0.9133</v>
+      </c>
+    </row>
+    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B29" s="38"/>
+      <c r="C29" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D29" s="16">
+        <v>100</v>
+      </c>
+      <c r="E29" s="16">
+        <v>83</v>
+      </c>
+      <c r="F29" s="17">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B30" s="37" t="s">
+        <v>31</v>
+      </c>
+      <c r="C30" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D30" s="16">
+        <v>150</v>
+      </c>
+      <c r="E30" s="16">
+        <v>137</v>
+      </c>
+      <c r="F30" s="17">
+        <v>0.9133</v>
+      </c>
+    </row>
+    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B31" s="38"/>
+      <c r="C31" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D31" s="16">
+        <v>100</v>
+      </c>
+      <c r="E31" s="16">
+        <v>84</v>
+      </c>
+      <c r="F31" s="17">
+        <v>0.84</v>
+      </c>
+    </row>
+    <row r="32" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B32" s="37" t="s">
+        <v>32</v>
+      </c>
+      <c r="C32" s="15" t="s">
+        <v>16</v>
+      </c>
+      <c r="D32" s="16">
+        <v>150</v>
+      </c>
+      <c r="E32" s="16">
+        <v>127</v>
+      </c>
+      <c r="F32" s="17">
+        <v>0.84670000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B33" s="38"/>
+      <c r="C33" s="15" t="s">
+        <v>15</v>
+      </c>
+      <c r="D33" s="16">
+        <v>100</v>
+      </c>
+      <c r="E33" s="16">
+        <v>75</v>
+      </c>
+      <c r="F33" s="17">
+        <v>0.75</v>
+      </c>
+    </row>
+    <row r="34" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B34" s="27" t="s">
         <v>27</v>
       </c>
-      <c r="C28" s="51" t="s">
+      <c r="C34" s="20" t="s">
         <v>16</v>
       </c>
-      <c r="D28" s="52">
-        <v>150</v>
-      </c>
-      <c r="E28" s="52">
+      <c r="D34" s="21">
+        <v>150</v>
+      </c>
+      <c r="E34" s="21">
         <v>119</v>
       </c>
-      <c r="F28" s="53">
+      <c r="F34" s="22">
         <v>0.79330000000000001</v>
       </c>
     </row>
-    <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="54"/>
-      <c r="C29" s="51" t="s">
+    <row r="35" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B35" s="28"/>
+      <c r="C35" s="20" t="s">
         <v>15</v>
       </c>
-      <c r="D29" s="52">
-        <v>100</v>
-      </c>
-      <c r="E29" s="52">
+      <c r="D35" s="21">
+        <v>100</v>
+      </c>
+      <c r="E35" s="21">
         <v>83</v>
       </c>
-      <c r="F29" s="53">
+      <c r="F35" s="22">
         <v>0.83</v>
       </c>
     </row>
-    <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="55" t="s">
+    <row r="36" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B36" s="27" t="s">
+        <v>35</v>
+      </c>
+      <c r="C36" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D36" s="21">
+        <v>150</v>
+      </c>
+      <c r="E36" s="21">
+        <v>132</v>
+      </c>
+      <c r="F36" s="22">
+        <v>0.88</v>
+      </c>
+    </row>
+    <row r="37" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B37" s="28"/>
+      <c r="C37" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D37" s="21">
+        <v>100</v>
+      </c>
+      <c r="E37" s="21">
+        <v>85</v>
+      </c>
+      <c r="F37" s="22">
+        <v>0.85</v>
+      </c>
+    </row>
+    <row r="38" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B38" s="29" t="s">
         <v>28</v>
       </c>
-      <c r="C30" s="56" t="s">
+      <c r="C38" s="23" t="s">
         <v>16</v>
       </c>
-      <c r="D30" s="57">
-        <v>150</v>
-      </c>
-      <c r="E30" s="57">
+      <c r="D38" s="24">
+        <v>150</v>
+      </c>
+      <c r="E38" s="24">
         <v>112</v>
       </c>
-      <c r="F30" s="58">
+      <c r="F38" s="25">
         <v>0.74670000000000003</v>
       </c>
     </row>
-    <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="59"/>
-      <c r="C31" s="56" t="s">
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="30"/>
+      <c r="C39" s="23" t="s">
         <v>15</v>
       </c>
-      <c r="D31" s="57">
-        <v>100</v>
-      </c>
-      <c r="E31" s="57">
+      <c r="D39" s="24">
+        <v>100</v>
+      </c>
+      <c r="E39" s="24">
         <v>86</v>
       </c>
-      <c r="F31" s="58">
+      <c r="F39" s="25">
         <v>0.86</v>
       </c>
     </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="29" t="s">
+        <v>36</v>
+      </c>
+      <c r="C40" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D40" s="24">
+        <v>150</v>
+      </c>
+      <c r="E40" s="24">
+        <v>131</v>
+      </c>
+      <c r="F40" s="25">
+        <v>0.87329999999999997</v>
+      </c>
+    </row>
+    <row r="41" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B41" s="30"/>
+      <c r="C41" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D41" s="24">
+        <v>100</v>
+      </c>
+      <c r="E41" s="24">
+        <v>84</v>
+      </c>
+      <c r="F41" s="25">
+        <v>0.84</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="15">
+  <mergeCells count="20">
+    <mergeCell ref="B40:B41"/>
     <mergeCell ref="B28:B29"/>
     <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B38:B39"/>
     <mergeCell ref="B12:B13"/>
     <mergeCell ref="C2:F2"/>
     <mergeCell ref="B4:B5"/>
@@ -3217,8 +3788,9 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
+    <mergeCell ref="B36:B37"/>
   </mergeCells>
-  <phoneticPr fontId="3" type="noConversion"/>
+  <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -3240,11 +3812,11 @@
     <row r="1" spans="2:5" ht="17" thickBot="1" x14ac:dyDescent="0.25"/>
     <row r="2" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B2" s="1"/>
-      <c r="C2" s="45" t="s">
+      <c r="C2" s="34" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="46"/>
-      <c r="E2" s="47"/>
+      <c r="D2" s="35"/>
+      <c r="E2" s="36"/>
     </row>
     <row r="3" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B3" s="2"/>
@@ -3310,16 +3882,16 @@
   <sheetData>
     <row r="2" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="31" t="s">
+      <c r="C2" s="26" t="s">
         <v>4</v>
       </c>
-      <c r="D2" s="31"/>
-      <c r="E2" s="31"/>
-      <c r="F2" s="31" t="s">
+      <c r="D2" s="26"/>
+      <c r="E2" s="26"/>
+      <c r="F2" s="26" t="s">
         <v>3</v>
       </c>
-      <c r="G2" s="31"/>
-      <c r="H2" s="31"/>
+      <c r="G2" s="26"/>
+      <c r="H2" s="26"/>
     </row>
     <row r="3" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>

</xml_diff>

<commit_message>
deepseek sqlcoder v2 eval
</commit_message>
<xml_diff>
--- a/evaluation/results_by_data_split.xlsx
+++ b/evaluation/results_by_data_split.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/yufeizhao/Desktop/11667MiniProject/11667-NLP2SQL/evaluation/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EDC2135B-B028-AE4E-91AA-CCC1785C1F30}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D7C1B4A9-BE0E-8242-B19D-B07699E78705}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-360" yWindow="-21820" windowWidth="28040" windowHeight="19460" activeTab="7" xr2:uid="{44081516-0D10-9B41-9157-44A5B55A14F9}"/>
+    <workbookView xWindow="-360" yWindow="-21820" windowWidth="28040" windowHeight="19460" activeTab="5" xr2:uid="{44081516-0D10-9B41-9157-44A5B55A14F9}"/>
   </bookViews>
   <sheets>
     <sheet name="train_sql2sql" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="217" uniqueCount="35">
   <si>
     <t>total queries</t>
   </si>
@@ -142,6 +142,12 @@
   </si>
   <si>
     <t>promptv4_sqlcoder_v1</t>
+  </si>
+  <si>
+    <t>promptv4_deepseek_v2</t>
+  </si>
+  <si>
+    <t>promptv4_sqlcoder_v2</t>
   </si>
 </sst>
 </file>
@@ -481,22 +487,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -506,6 +500,18 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="5" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="12" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="13" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
@@ -1029,10 +1035,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{274C775F-3A5B-8346-B68B-D75012605A96}">
-  <dimension ref="B2:H24"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
     <sheetView zoomScale="157" workbookViewId="0">
-      <selection activeCell="B24" sqref="B24"/>
+      <selection activeCell="E10" sqref="E10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1514,48 +1520,94 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C23" s="3">
         <v>250</v>
       </c>
       <c r="D23" s="3">
-        <v>3</v>
+        <v>134</v>
       </c>
       <c r="E23" s="10">
-        <v>1.2E-2</v>
+        <v>0.53600000000000003</v>
       </c>
       <c r="F23" s="3">
         <v>250</v>
       </c>
       <c r="G23" s="3">
-        <v>2292</v>
+        <v>789</v>
       </c>
       <c r="H23" s="3">
-        <v>9.17</v>
+        <v>3.16</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3">
+        <v>250</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="10">
+        <v>1.2E-2</v>
+      </c>
+      <c r="F24" s="3">
+        <v>250</v>
+      </c>
+      <c r="G24" s="3">
+        <v>2292</v>
+      </c>
+      <c r="H24" s="3">
+        <v>9.17</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="3">
-        <v>250</v>
-      </c>
-      <c r="D24" s="3">
+      <c r="C25" s="3">
+        <v>250</v>
+      </c>
+      <c r="D25" s="3">
         <v>115</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E25" s="10">
         <v>0.46</v>
       </c>
-      <c r="F24" s="3">
-        <v>250</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="F25" s="3">
+        <v>250</v>
+      </c>
+      <c r="G25" s="3">
         <v>904</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H25" s="3">
         <v>3.62</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="3">
+        <v>250</v>
+      </c>
+      <c r="D26" s="3">
+        <v>133</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0.53200000000000003</v>
+      </c>
+      <c r="F26" s="3">
+        <v>250</v>
+      </c>
+      <c r="G26" s="3">
+        <v>776</v>
+      </c>
+      <c r="H26" s="12">
+        <v>3.1</v>
       </c>
     </row>
   </sheetData>
@@ -1570,10 +1622,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F82A48FE-26B2-E846-83D1-3D5B61BC4083}">
-  <dimension ref="B2:H24"/>
+  <dimension ref="B2:H26"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="D10" sqref="D10"/>
+      <selection activeCell="J15" sqref="J15:J16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2055,48 +2107,94 @@
     </row>
     <row r="23" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B23" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C23" s="3">
         <v>250</v>
       </c>
       <c r="D23" s="3">
-        <v>2</v>
+        <v>138</v>
       </c>
       <c r="E23" s="10">
-        <v>8.0000000000000002E-3</v>
+        <v>0.55200000000000005</v>
       </c>
       <c r="F23" s="3">
         <v>250</v>
       </c>
       <c r="G23" s="3">
-        <v>2273</v>
+        <v>839</v>
       </c>
       <c r="H23" s="3">
-        <v>9.09</v>
+        <v>3.36</v>
       </c>
     </row>
     <row r="24" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B24" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C24" s="3">
+        <v>250</v>
+      </c>
+      <c r="D24" s="3">
+        <v>2</v>
+      </c>
+      <c r="E24" s="10">
+        <v>8.0000000000000002E-3</v>
+      </c>
+      <c r="F24" s="3">
+        <v>250</v>
+      </c>
+      <c r="G24" s="3">
+        <v>2273</v>
+      </c>
+      <c r="H24" s="3">
+        <v>9.09</v>
+      </c>
+    </row>
+    <row r="25" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B25" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C24" s="3">
-        <v>250</v>
-      </c>
-      <c r="D24" s="3">
+      <c r="C25" s="3">
+        <v>250</v>
+      </c>
+      <c r="D25" s="3">
         <v>123</v>
       </c>
-      <c r="E24" s="10">
+      <c r="E25" s="10">
         <v>0.49199999999999999</v>
       </c>
-      <c r="F24" s="3">
-        <v>250</v>
-      </c>
-      <c r="G24" s="3">
+      <c r="F25" s="3">
+        <v>250</v>
+      </c>
+      <c r="G25" s="3">
         <v>910</v>
       </c>
-      <c r="H24" s="3">
+      <c r="H25" s="3">
         <v>3.64</v>
+      </c>
+    </row>
+    <row r="26" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B26" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C26" s="3">
+        <v>250</v>
+      </c>
+      <c r="D26" s="3">
+        <v>139</v>
+      </c>
+      <c r="E26" s="10">
+        <v>0.55600000000000005</v>
+      </c>
+      <c r="F26" s="3">
+        <v>250</v>
+      </c>
+      <c r="G26" s="3">
+        <v>801</v>
+      </c>
+      <c r="H26" s="12">
+        <v>3.2</v>
       </c>
     </row>
   </sheetData>
@@ -2111,10 +2209,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{EA613D23-B9DE-0542-95AA-364F896410C8}">
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView zoomScale="150" workbookViewId="0">
-      <selection activeCell="B14" sqref="B14"/>
+      <selection activeCell="J25" sqref="J25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2550,48 +2648,94 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3">
         <v>150</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>25</v>
       </c>
       <c r="E21" s="10">
-        <v>0</v>
+        <v>0.16669999999999999</v>
       </c>
       <c r="F21" s="3">
         <v>150</v>
       </c>
       <c r="G21" s="3">
-        <v>1728</v>
+        <v>456</v>
       </c>
       <c r="H21" s="3">
-        <v>11.52</v>
+        <v>3.04</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3">
+        <v>150</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>150</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1728</v>
+      </c>
+      <c r="H22" s="3">
+        <v>11.52</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="3">
-        <v>150</v>
-      </c>
-      <c r="D22" s="3">
+      <c r="C23" s="3">
+        <v>150</v>
+      </c>
+      <c r="D23" s="3">
         <v>10</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="10">
         <v>6.6699999999999995E-2</v>
       </c>
-      <c r="F22" s="3">
-        <v>150</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F23" s="3">
+        <v>150</v>
+      </c>
+      <c r="G23" s="3">
         <v>772</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H23" s="3">
         <v>5.15</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="3">
+        <v>150</v>
+      </c>
+      <c r="D24" s="3">
+        <v>25</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.16669999999999999</v>
+      </c>
+      <c r="F24" s="3">
+        <v>150</v>
+      </c>
+      <c r="G24" s="3">
+        <v>406</v>
+      </c>
+      <c r="H24" s="3">
+        <v>2.71</v>
       </c>
     </row>
   </sheetData>
@@ -2606,10 +2750,10 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{06C74F51-BDAD-924D-AEFA-68C8E4D340A8}">
-  <dimension ref="B2:H22"/>
+  <dimension ref="B2:H24"/>
   <sheetViews>
     <sheetView zoomScale="138" workbookViewId="0">
-      <selection activeCell="C22" sqref="C22"/>
+      <selection activeCell="I28" sqref="I28:I29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3045,48 +3189,94 @@
     </row>
     <row r="21" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B21" s="3" t="s">
-        <v>26</v>
+        <v>33</v>
       </c>
       <c r="C21" s="3">
         <v>100</v>
       </c>
       <c r="D21" s="3">
-        <v>0</v>
+        <v>7</v>
       </c>
       <c r="E21" s="10">
-        <v>0</v>
+        <v>7.0000000000000007E-2</v>
       </c>
       <c r="F21" s="3">
         <v>100</v>
       </c>
       <c r="G21" s="3">
-        <v>1021</v>
+        <v>672</v>
       </c>
       <c r="H21" s="3">
-        <v>10.210000000000001</v>
+        <v>6.72</v>
       </c>
     </row>
     <row r="22" spans="2:8" x14ac:dyDescent="0.2">
       <c r="B22" s="3" t="s">
+        <v>26</v>
+      </c>
+      <c r="C22" s="3">
+        <v>100</v>
+      </c>
+      <c r="D22" s="3">
+        <v>0</v>
+      </c>
+      <c r="E22" s="10">
+        <v>0</v>
+      </c>
+      <c r="F22" s="3">
+        <v>100</v>
+      </c>
+      <c r="G22" s="3">
+        <v>1021</v>
+      </c>
+      <c r="H22" s="3">
+        <v>10.210000000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B23" s="3" t="s">
         <v>32</v>
       </c>
-      <c r="C22" s="3">
-        <v>100</v>
-      </c>
-      <c r="D22" s="3">
+      <c r="C23" s="3">
+        <v>100</v>
+      </c>
+      <c r="D23" s="3">
         <v>4</v>
       </c>
-      <c r="E22" s="10">
+      <c r="E23" s="10">
         <v>0.04</v>
       </c>
-      <c r="F22" s="3">
-        <v>100</v>
-      </c>
-      <c r="G22" s="3">
+      <c r="F23" s="3">
+        <v>100</v>
+      </c>
+      <c r="G23" s="3">
         <v>655</v>
       </c>
-      <c r="H22" s="3">
+      <c r="H23" s="3">
         <v>6.55</v>
+      </c>
+    </row>
+    <row r="24" spans="2:8" x14ac:dyDescent="0.2">
+      <c r="B24" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="C24" s="3">
+        <v>100</v>
+      </c>
+      <c r="D24" s="3">
+        <v>3</v>
+      </c>
+      <c r="E24" s="10">
+        <v>0.03</v>
+      </c>
+      <c r="F24" s="3">
+        <v>100</v>
+      </c>
+      <c r="G24" s="3">
+        <v>674</v>
+      </c>
+      <c r="H24" s="3">
+        <v>6.74</v>
       </c>
     </row>
   </sheetData>
@@ -3101,10 +3291,10 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D15506EA-4930-9441-B4F3-EDD7A1FF6E26}">
-  <dimension ref="B2:F41"/>
+  <dimension ref="B2:F45"/>
   <sheetViews>
-    <sheetView topLeftCell="A13" zoomScale="125" workbookViewId="0">
-      <selection activeCell="F27" sqref="F27"/>
+    <sheetView tabSelected="1" topLeftCell="A16" zoomScale="125" workbookViewId="0">
+      <selection activeCell="H46" sqref="H46"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -3116,12 +3306,12 @@
   <sheetData>
     <row r="2" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B2" s="3"/>
-      <c r="C2" s="36" t="s">
+      <c r="C2" s="32" t="s">
         <v>8</v>
       </c>
-      <c r="D2" s="36"/>
-      <c r="E2" s="36"/>
-      <c r="F2" s="36"/>
+      <c r="D2" s="32"/>
+      <c r="E2" s="32"/>
+      <c r="F2" s="32"/>
     </row>
     <row r="3" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B3" s="3"/>
@@ -3139,7 +3329,7 @@
       </c>
     </row>
     <row r="4" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B4" s="37" t="s">
+      <c r="B4" s="33" t="s">
         <v>11</v>
       </c>
       <c r="C4" s="26" t="s">
@@ -3156,7 +3346,7 @@
       </c>
     </row>
     <row r="5" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B5" s="38"/>
+      <c r="B5" s="34"/>
       <c r="C5" s="26" t="s">
         <v>15</v>
       </c>
@@ -3171,7 +3361,7 @@
       </c>
     </row>
     <row r="6" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B6" s="37" t="s">
+      <c r="B6" s="33" t="s">
         <v>12</v>
       </c>
       <c r="C6" s="26" t="s">
@@ -3188,7 +3378,7 @@
       </c>
     </row>
     <row r="7" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B7" s="38"/>
+      <c r="B7" s="34"/>
       <c r="C7" s="26" t="s">
         <v>15</v>
       </c>
@@ -3203,7 +3393,7 @@
       </c>
     </row>
     <row r="8" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B8" s="37" t="s">
+      <c r="B8" s="33" t="s">
         <v>13</v>
       </c>
       <c r="C8" s="26" t="s">
@@ -3220,7 +3410,7 @@
       </c>
     </row>
     <row r="9" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B9" s="38"/>
+      <c r="B9" s="34"/>
       <c r="C9" s="26" t="s">
         <v>15</v>
       </c>
@@ -3235,7 +3425,7 @@
       </c>
     </row>
     <row r="10" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B10" s="37" t="s">
+      <c r="B10" s="33" t="s">
         <v>14</v>
       </c>
       <c r="C10" s="26" t="s">
@@ -3252,7 +3442,7 @@
       </c>
     </row>
     <row r="11" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B11" s="38"/>
+      <c r="B11" s="34"/>
       <c r="C11" s="26" t="s">
         <v>15</v>
       </c>
@@ -3267,7 +3457,7 @@
       </c>
     </row>
     <row r="12" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B12" s="32" t="s">
+      <c r="B12" s="30" t="s">
         <v>27</v>
       </c>
       <c r="C12" s="15" t="s">
@@ -3284,7 +3474,7 @@
       </c>
     </row>
     <row r="13" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B13" s="33"/>
+      <c r="B13" s="31"/>
       <c r="C13" s="15" t="s">
         <v>15</v>
       </c>
@@ -3299,7 +3489,7 @@
       </c>
     </row>
     <row r="14" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B14" s="32" t="s">
+      <c r="B14" s="30" t="s">
         <v>18</v>
       </c>
       <c r="C14" s="15" t="s">
@@ -3316,7 +3506,7 @@
       </c>
     </row>
     <row r="15" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B15" s="33"/>
+      <c r="B15" s="31"/>
       <c r="C15" s="15" t="s">
         <v>15</v>
       </c>
@@ -3331,7 +3521,7 @@
       </c>
     </row>
     <row r="16" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B16" s="32" t="s">
+      <c r="B16" s="30" t="s">
         <v>19</v>
       </c>
       <c r="C16" s="15" t="s">
@@ -3348,7 +3538,7 @@
       </c>
     </row>
     <row r="17" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B17" s="33"/>
+      <c r="B17" s="31"/>
       <c r="C17" s="15" t="s">
         <v>15</v>
       </c>
@@ -3363,7 +3553,7 @@
       </c>
     </row>
     <row r="18" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B18" s="32" t="s">
+      <c r="B18" s="30" t="s">
         <v>20</v>
       </c>
       <c r="C18" s="15" t="s">
@@ -3380,7 +3570,7 @@
       </c>
     </row>
     <row r="19" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B19" s="33"/>
+      <c r="B19" s="31"/>
       <c r="C19" s="15" t="s">
         <v>15</v>
       </c>
@@ -3395,7 +3585,7 @@
       </c>
     </row>
     <row r="20" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B20" s="32" t="s">
+      <c r="B20" s="30" t="s">
         <v>21</v>
       </c>
       <c r="C20" s="15" t="s">
@@ -3412,7 +3602,7 @@
       </c>
     </row>
     <row r="21" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B21" s="33"/>
+      <c r="B21" s="31"/>
       <c r="C21" s="15" t="s">
         <v>15</v>
       </c>
@@ -3427,7 +3617,7 @@
       </c>
     </row>
     <row r="22" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B22" s="32" t="s">
+      <c r="B22" s="30" t="s">
         <v>22</v>
       </c>
       <c r="C22" s="15" t="s">
@@ -3444,7 +3634,7 @@
       </c>
     </row>
     <row r="23" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B23" s="33"/>
+      <c r="B23" s="31"/>
       <c r="C23" s="15" t="s">
         <v>15</v>
       </c>
@@ -3459,7 +3649,7 @@
       </c>
     </row>
     <row r="24" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B24" s="32" t="s">
+      <c r="B24" s="30" t="s">
         <v>23</v>
       </c>
       <c r="C24" s="15" t="s">
@@ -3476,7 +3666,7 @@
       </c>
     </row>
     <row r="25" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B25" s="33"/>
+      <c r="B25" s="31"/>
       <c r="C25" s="15" t="s">
         <v>15</v>
       </c>
@@ -3491,7 +3681,7 @@
       </c>
     </row>
     <row r="26" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B26" s="32" t="s">
+      <c r="B26" s="30" t="s">
         <v>24</v>
       </c>
       <c r="C26" s="15" t="s">
@@ -3508,7 +3698,7 @@
       </c>
     </row>
     <row r="27" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B27" s="33"/>
+      <c r="B27" s="31"/>
       <c r="C27" s="15" t="s">
         <v>15</v>
       </c>
@@ -3523,7 +3713,7 @@
       </c>
     </row>
     <row r="28" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B28" s="32" t="s">
+      <c r="B28" s="30" t="s">
         <v>28</v>
       </c>
       <c r="C28" s="15" t="s">
@@ -3540,7 +3730,7 @@
       </c>
     </row>
     <row r="29" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B29" s="33"/>
+      <c r="B29" s="31"/>
       <c r="C29" s="15" t="s">
         <v>15</v>
       </c>
@@ -3555,7 +3745,7 @@
       </c>
     </row>
     <row r="30" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B30" s="32" t="s">
+      <c r="B30" s="30" t="s">
         <v>29</v>
       </c>
       <c r="C30" s="15" t="s">
@@ -3572,7 +3762,7 @@
       </c>
     </row>
     <row r="31" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B31" s="33"/>
+      <c r="B31" s="31"/>
       <c r="C31" s="15" t="s">
         <v>15</v>
       </c>
@@ -3587,7 +3777,7 @@
       </c>
     </row>
     <row r="32" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B32" s="32" t="s">
+      <c r="B32" s="30" t="s">
         <v>30</v>
       </c>
       <c r="C32" s="15" t="s">
@@ -3604,7 +3794,7 @@
       </c>
     </row>
     <row r="33" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B33" s="33"/>
+      <c r="B33" s="31"/>
       <c r="C33" s="15" t="s">
         <v>15</v>
       </c>
@@ -3619,7 +3809,7 @@
       </c>
     </row>
     <row r="34" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B34" s="34" t="s">
+      <c r="B34" s="37" t="s">
         <v>25</v>
       </c>
       <c r="C34" s="20" t="s">
@@ -3636,7 +3826,7 @@
       </c>
     </row>
     <row r="35" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B35" s="35"/>
+      <c r="B35" s="38"/>
       <c r="C35" s="20" t="s">
         <v>15</v>
       </c>
@@ -3651,7 +3841,7 @@
       </c>
     </row>
     <row r="36" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B36" s="34" t="s">
+      <c r="B36" s="37" t="s">
         <v>31</v>
       </c>
       <c r="C36" s="20" t="s">
@@ -3668,7 +3858,7 @@
       </c>
     </row>
     <row r="37" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B37" s="35"/>
+      <c r="B37" s="38"/>
       <c r="C37" s="20" t="s">
         <v>15</v>
       </c>
@@ -3683,40 +3873,40 @@
       </c>
     </row>
     <row r="38" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B38" s="30" t="s">
+      <c r="B38" s="37" t="s">
+        <v>33</v>
+      </c>
+      <c r="C38" s="20" t="s">
+        <v>16</v>
+      </c>
+      <c r="D38" s="21">
+        <v>150</v>
+      </c>
+      <c r="E38" s="21">
+        <v>137</v>
+      </c>
+      <c r="F38" s="22">
+        <v>0.9133</v>
+      </c>
+    </row>
+    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B39" s="38"/>
+      <c r="C39" s="20" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39" s="21">
+        <v>100</v>
+      </c>
+      <c r="E39" s="21">
+        <v>91</v>
+      </c>
+      <c r="F39" s="22">
+        <v>0.91</v>
+      </c>
+    </row>
+    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B40" s="35" t="s">
         <v>26</v>
-      </c>
-      <c r="C38" s="23" t="s">
-        <v>16</v>
-      </c>
-      <c r="D38" s="24">
-        <v>150</v>
-      </c>
-      <c r="E38" s="24">
-        <v>112</v>
-      </c>
-      <c r="F38" s="25">
-        <v>0.74670000000000003</v>
-      </c>
-    </row>
-    <row r="39" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B39" s="31"/>
-      <c r="C39" s="23" t="s">
-        <v>15</v>
-      </c>
-      <c r="D39" s="24">
-        <v>100</v>
-      </c>
-      <c r="E39" s="24">
-        <v>86</v>
-      </c>
-      <c r="F39" s="25">
-        <v>0.86</v>
-      </c>
-    </row>
-    <row r="40" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B40" s="30" t="s">
-        <v>32</v>
       </c>
       <c r="C40" s="23" t="s">
         <v>16</v>
@@ -3725,14 +3915,14 @@
         <v>150</v>
       </c>
       <c r="E40" s="24">
-        <v>131</v>
+        <v>112</v>
       </c>
       <c r="F40" s="25">
-        <v>0.87329999999999997</v>
+        <v>0.74670000000000003</v>
       </c>
     </row>
     <row r="41" spans="2:6" x14ac:dyDescent="0.2">
-      <c r="B41" s="31"/>
+      <c r="B41" s="36"/>
       <c r="C41" s="23" t="s">
         <v>15</v>
       </c>
@@ -3740,14 +3930,93 @@
         <v>100</v>
       </c>
       <c r="E41" s="24">
+        <v>86</v>
+      </c>
+      <c r="F41" s="25">
+        <v>0.86</v>
+      </c>
+    </row>
+    <row r="42" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B42" s="35" t="s">
+        <v>32</v>
+      </c>
+      <c r="C42" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D42" s="24">
+        <v>150</v>
+      </c>
+      <c r="E42" s="24">
+        <v>131</v>
+      </c>
+      <c r="F42" s="25">
+        <v>0.87329999999999997</v>
+      </c>
+    </row>
+    <row r="43" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B43" s="36"/>
+      <c r="C43" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D43" s="24">
+        <v>100</v>
+      </c>
+      <c r="E43" s="24">
         <v>84</v>
       </c>
-      <c r="F41" s="25">
+      <c r="F43" s="25">
         <v>0.84</v>
       </c>
     </row>
+    <row r="44" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B44" s="35" t="s">
+        <v>34</v>
+      </c>
+      <c r="C44" s="23" t="s">
+        <v>16</v>
+      </c>
+      <c r="D44" s="24">
+        <v>150</v>
+      </c>
+      <c r="E44" s="24">
+        <v>137</v>
+      </c>
+      <c r="F44" s="25">
+        <v>0.9133</v>
+      </c>
+    </row>
+    <row r="45" spans="2:6" x14ac:dyDescent="0.2">
+      <c r="B45" s="36"/>
+      <c r="C45" s="23" t="s">
+        <v>15</v>
+      </c>
+      <c r="D45" s="24">
+        <v>100</v>
+      </c>
+      <c r="E45" s="24">
+        <v>76</v>
+      </c>
+      <c r="F45" s="25">
+        <v>0.76</v>
+      </c>
+    </row>
   </sheetData>
-  <mergeCells count="20">
+  <mergeCells count="22">
+    <mergeCell ref="B44:B45"/>
+    <mergeCell ref="B42:B43"/>
+    <mergeCell ref="B28:B29"/>
+    <mergeCell ref="B30:B31"/>
+    <mergeCell ref="B32:B33"/>
+    <mergeCell ref="B34:B35"/>
+    <mergeCell ref="B40:B41"/>
+    <mergeCell ref="B36:B37"/>
+    <mergeCell ref="B38:B39"/>
+    <mergeCell ref="B12:B13"/>
+    <mergeCell ref="C2:F2"/>
+    <mergeCell ref="B4:B5"/>
+    <mergeCell ref="B6:B7"/>
+    <mergeCell ref="B8:B9"/>
+    <mergeCell ref="B10:B11"/>
     <mergeCell ref="B26:B27"/>
     <mergeCell ref="B14:B15"/>
     <mergeCell ref="B16:B17"/>
@@ -3755,19 +4024,6 @@
     <mergeCell ref="B20:B21"/>
     <mergeCell ref="B22:B23"/>
     <mergeCell ref="B24:B25"/>
-    <mergeCell ref="B12:B13"/>
-    <mergeCell ref="C2:F2"/>
-    <mergeCell ref="B4:B5"/>
-    <mergeCell ref="B6:B7"/>
-    <mergeCell ref="B8:B9"/>
-    <mergeCell ref="B10:B11"/>
-    <mergeCell ref="B40:B41"/>
-    <mergeCell ref="B28:B29"/>
-    <mergeCell ref="B30:B31"/>
-    <mergeCell ref="B32:B33"/>
-    <mergeCell ref="B34:B35"/>
-    <mergeCell ref="B38:B39"/>
-    <mergeCell ref="B36:B37"/>
   </mergeCells>
   <phoneticPr fontId="2" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3849,7 +4105,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{BF9F312D-430D-0042-B1CF-DB1A21B73BB7}">
   <dimension ref="B2:H5"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="159" workbookViewId="0">
+    <sheetView zoomScale="159" workbookViewId="0">
       <selection activeCell="F21" sqref="F21"/>
     </sheetView>
   </sheetViews>

</xml_diff>